<commit_message>
Auto-committed on 2022/04/19 週二
</commit_message>
<xml_diff>
--- a/Program/Other/LM057_底稿_表14-5、14-6_會計部申報表.xlsx
+++ b/Program/Other/LM057_底稿_表14-5、14-6_會計部申報表.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5952" yWindow="120" windowWidth="6000" windowHeight="6408" tabRatio="853" activeTab="2"/>
+    <workbookView xWindow="5950" yWindow="120" windowWidth="6000" windowHeight="6410" tabRatio="853" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="表14-6" sheetId="4" r:id="rId1"/>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="97">
   <si>
     <t>i.其他非屬催收款之逾期放款</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -326,18 +326,7 @@
     <t>序號</t>
   </si>
   <si>
-    <t>到期 日</t>
-  </si>
-  <si>
     <t>分類</t>
-  </si>
-  <si>
-    <t>法務進度_C5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C7</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>分配不足額C5-B3</t>
@@ -1231,6 +1220,26 @@
   </si>
   <si>
     <t>C7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>繳息迄日</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>利率</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>法務進度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>利率代碼</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶號額度</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1238,14 +1247,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="#,##0_ "/>
     <numFmt numFmtId="177" formatCode="0.000%"/>
     <numFmt numFmtId="178" formatCode="#,##0_);[Red]\(#,##0\)"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="181" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="182" formatCode="0.000_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1450,7 +1460,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1644,7 +1654,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1708,30 +1718,12 @@
     <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="14" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="14" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1745,18 +1737,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1814,9 +1797,6 @@
     <xf numFmtId="180" fontId="18" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1933,6 +1913,60 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="14" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="1" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2311,16 +2345,16 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" style="4" customWidth="1"/>
     <col min="3" max="3" width="45" style="4" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.90625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.8">
+    <row r="1" spans="1:4" ht="19.5">
       <c r="A1" s="7"/>
       <c r="B1" s="15" t="s">
         <v>36</v>
@@ -2330,7 +2364,7 @@
       </c>
       <c r="D1" s="13"/>
     </row>
-    <row r="2" spans="1:4" ht="19.8">
+    <row r="2" spans="1:4" ht="19.5">
       <c r="A2" s="7"/>
       <c r="B2" s="13"/>
       <c r="C2" s="10" t="s">
@@ -2341,7 +2375,7 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.8">
+    <row r="3" spans="1:4" ht="19.5">
       <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
@@ -2351,23 +2385,23 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="19.8">
+    <row r="4" spans="1:4" ht="19.5">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="79"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="19.8">
+    <row r="5" spans="1:4" ht="19.5">
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="70" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2379,67 +2413,67 @@
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="81"/>
+      <c r="B6" s="71"/>
       <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="19.8">
+    <row r="7" spans="1:4" ht="19.5">
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="81"/>
+      <c r="B7" s="71"/>
       <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="19.8">
+    <row r="8" spans="1:4" ht="19.5">
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="81"/>
+      <c r="B8" s="71"/>
       <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="19.8">
+    <row r="9" spans="1:4" ht="19.5">
       <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" s="81"/>
+      <c r="B9" s="71"/>
       <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="19.8">
+    <row r="10" spans="1:4" ht="19.5">
       <c r="A10" s="1">
         <v>6</v>
       </c>
-      <c r="B10" s="81"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="19.8">
+    <row r="11" spans="1:4" ht="19.5">
       <c r="A11" s="1">
         <v>7</v>
       </c>
-      <c r="B11" s="81"/>
+      <c r="B11" s="71"/>
       <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="19.8">
+    <row r="12" spans="1:4" ht="19.5">
       <c r="A12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="73" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -2450,11 +2484,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="19.8">
+    <row r="13" spans="1:4" ht="19.5">
       <c r="A13" s="1">
         <v>9</v>
       </c>
-      <c r="B13" s="84"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="12" t="s">
         <v>0</v>
       </c>
@@ -2463,11 +2497,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="19.8">
+    <row r="14" spans="1:4" ht="19.5">
       <c r="A14" s="1">
         <v>10</v>
       </c>
-      <c r="B14" s="85"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="12" t="s">
         <v>1</v>
       </c>
@@ -2476,60 +2510,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="19.8">
+    <row r="15" spans="1:4" ht="19.5">
       <c r="A15" s="1">
         <v>11</v>
       </c>
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="82"/>
+      <c r="C15" s="72"/>
       <c r="D15" s="17">
         <f>'14-5申報表'!D18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="19.8">
+    <row r="16" spans="1:4" ht="19.5">
       <c r="A16" s="1">
         <v>12</v>
       </c>
-      <c r="B16" s="86" t="s">
+      <c r="B16" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="87"/>
+      <c r="C16" s="77"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:5" ht="39" customHeight="1">
       <c r="A17" s="1">
         <v>13</v>
       </c>
-      <c r="B17" s="88" t="s">
+      <c r="B17" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="89"/>
+      <c r="C17" s="79"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:5" ht="39" customHeight="1">
       <c r="A18" s="1">
         <v>14</v>
       </c>
-      <c r="B18" s="88" t="s">
+      <c r="B18" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="89"/>
+      <c r="C18" s="79"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="19.8">
+    <row r="19" spans="1:5" ht="19.5">
       <c r="A19" s="1">
         <v>15</v>
       </c>
-      <c r="B19" s="86" t="s">
+      <c r="B19" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="87"/>
+      <c r="C19" s="77"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="19.8">
+    <row r="20" spans="1:5" ht="19.5">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -2542,7 +2576,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="19.8">
+    <row r="21" spans="1:5" ht="19.5">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -2556,23 +2590,23 @@
       <c r="A22" s="1">
         <v>18</v>
       </c>
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="80"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:5" ht="36" customHeight="1">
       <c r="A23" s="1">
         <v>19</v>
       </c>
-      <c r="B23" s="80" t="s">
+      <c r="B23" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="80"/>
+      <c r="C23" s="70"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:5" ht="19.8">
+    <row r="24" spans="1:5" ht="19.5">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -2657,350 +2691,350 @@
   </sheetPr>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" customWidth="1"/>
     <col min="3" max="3" width="54" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" style="19" customWidth="1"/>
     <col min="5" max="5" width="4" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.36328125" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.8">
-      <c r="A1" s="76"/>
+    <row r="1" spans="1:7" ht="19.5">
+      <c r="A1" s="66"/>
       <c r="B1" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="75"/>
-    </row>
-    <row r="2" spans="1:7" ht="17.399999999999999">
-      <c r="A2" s="76"/>
-      <c r="B2" s="75"/>
+      <c r="D1" s="65"/>
+    </row>
+    <row r="2" spans="1:7" ht="17.5">
+      <c r="A2" s="66"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="74">
+        <v>86</v>
+      </c>
+      <c r="D2" s="64">
         <v>43585</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="92" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="93"/>
-      <c r="D4" s="73" t="s">
+      <c r="B4" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="83"/>
+      <c r="D4" s="63" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="32.4">
-      <c r="A5" s="52">
+    <row r="5" spans="1:7" ht="34">
+      <c r="A5" s="43">
         <v>1</v>
       </c>
-      <c r="B5" s="94" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="62" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="54"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="48"/>
-    </row>
-    <row r="6" spans="1:7" ht="32.4">
-      <c r="A6" s="52">
+      <c r="B5" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="45"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="39"/>
+    </row>
+    <row r="6" spans="1:7" ht="34">
+      <c r="A6" s="43">
         <v>2</v>
       </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="70"/>
-      <c r="F6" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="G6" s="48" t="s">
-        <v>61</v>
+      <c r="B6" s="85"/>
+      <c r="C6" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="60"/>
+      <c r="F6" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="26.4" customHeight="1">
-      <c r="A7" s="52">
+      <c r="A7" s="43">
         <v>3</v>
       </c>
-      <c r="B7" s="95"/>
-      <c r="C7" s="72" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="71"/>
-      <c r="F7" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="G7" s="69"/>
-    </row>
-    <row r="8" spans="1:7" ht="48.6">
-      <c r="A8" s="52">
+      <c r="B7" s="85"/>
+      <c r="C7" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="61"/>
+      <c r="F7" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="59"/>
+    </row>
+    <row r="8" spans="1:7" ht="34">
+      <c r="A8" s="43">
         <v>4</v>
       </c>
-      <c r="B8" s="95"/>
-      <c r="C8" s="67" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="70"/>
-      <c r="F8" s="78" t="s">
-        <v>92</v>
-      </c>
-      <c r="G8" s="77"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="60"/>
+      <c r="F8" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="67"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="52">
+      <c r="A9" s="43">
         <v>5</v>
       </c>
-      <c r="B9" s="95"/>
-      <c r="C9" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="58">
+      <c r="B9" s="85"/>
+      <c r="C9" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="48">
         <f>SUM(D5:D8)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="78" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" s="77"/>
-    </row>
-    <row r="10" spans="1:7" ht="32.4">
-      <c r="A10" s="52">
+      <c r="F9" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" s="67"/>
+    </row>
+    <row r="10" spans="1:7" ht="34">
+      <c r="A10" s="43">
         <v>6</v>
       </c>
-      <c r="B10" s="94" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="67" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="70"/>
-      <c r="F10" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="G10" s="69"/>
+      <c r="B10" s="84" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="60"/>
+      <c r="F10" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="59"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="52">
+      <c r="A11" s="43">
         <v>7</v>
       </c>
-      <c r="B11" s="96"/>
-      <c r="C11" s="67" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="57"/>
-      <c r="F11" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="68"/>
-    </row>
-    <row r="12" spans="1:7" ht="32.4">
-      <c r="A12" s="52">
+      <c r="B11" s="86"/>
+      <c r="C11" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="45"/>
+      <c r="F11" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="58"/>
+    </row>
+    <row r="12" spans="1:7" ht="34">
+      <c r="A12" s="43">
         <v>8</v>
       </c>
-      <c r="B12" s="96"/>
-      <c r="C12" s="67" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="63"/>
-      <c r="F12" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="66"/>
-    </row>
-    <row r="13" spans="1:7" ht="48.6">
-      <c r="A13" s="52">
+      <c r="B12" s="86"/>
+      <c r="C12" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="53"/>
+      <c r="F12" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="56"/>
+    </row>
+    <row r="13" spans="1:7" ht="51">
+      <c r="A13" s="43">
         <v>9</v>
       </c>
-      <c r="B13" s="96"/>
-      <c r="C13" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="63"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="60">
+      <c r="B13" s="86"/>
+      <c r="C13" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="53"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="50">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="52">
+      <c r="A14" s="43">
         <v>10</v>
       </c>
-      <c r="B14" s="96"/>
-      <c r="C14" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="54"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="60">
+      <c r="B14" s="86"/>
+      <c r="C14" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="45"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="50">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="32.4">
-      <c r="A15" s="52">
+    <row r="15" spans="1:7" ht="34">
+      <c r="A15" s="43">
         <v>11</v>
       </c>
-      <c r="B15" s="96"/>
-      <c r="C15" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="63"/>
-      <c r="F15" s="61" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="60">
+      <c r="B15" s="86"/>
+      <c r="C15" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="53"/>
+      <c r="F15" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="50">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="52">
+      <c r="A16" s="43">
         <v>12</v>
       </c>
-      <c r="B16" s="96"/>
-      <c r="C16" s="62" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="54"/>
-      <c r="F16" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" s="60">
+      <c r="B16" s="86"/>
+      <c r="C16" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="45"/>
+      <c r="F16" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="50">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="52">
+      <c r="A17" s="43">
         <v>13</v>
       </c>
-      <c r="B17" s="96"/>
-      <c r="C17" s="59" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="58">
+      <c r="B17" s="86"/>
+      <c r="C17" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="48">
         <f>SUM(D10:D16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="52">
+      <c r="A18" s="43">
         <v>14</v>
       </c>
-      <c r="B18" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="57"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="55"/>
+      <c r="B18" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="45"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="46"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="52">
+      <c r="A19" s="43">
         <v>15</v>
       </c>
-      <c r="B19" s="51" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="54">
+      <c r="B19" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="45">
         <f>D9+D17+G15+G16</f>
         <v>0</v>
       </c>
-      <c r="F19" s="53">
+      <c r="F19" s="44">
         <v>0</v>
       </c>
-      <c r="G19" s="53">
+      <c r="G19" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="52">
+      <c r="A20" s="43">
         <v>16</v>
       </c>
-      <c r="B20" s="51" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="50" t="e">
+      <c r="B20" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="41" t="e">
         <f>D9/D18</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="52">
+      <c r="A21" s="43">
         <v>17</v>
       </c>
-      <c r="B21" s="51" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="50" t="e">
+      <c r="B21" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="42"/>
+      <c r="D21" s="41" t="e">
         <f>D17/D18</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="52">
+      <c r="A22" s="43">
         <v>18</v>
       </c>
-      <c r="B22" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="50" t="e">
+      <c r="B22" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="41" t="e">
         <f>D19/D18</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F22" s="47"/>
-      <c r="G22" s="48"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="39"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
-      <c r="F23" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="48" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="45" customFormat="1">
-      <c r="A24" s="90" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="91"/>
-      <c r="C24" s="91"/>
-      <c r="D24" s="91"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="46"/>
+      <c r="F23" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="36" customFormat="1">
+      <c r="A24" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="81"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="37"/>
       <c r="H24"/>
       <c r="I24"/>
       <c r="J24"/>
@@ -3009,51 +3043,51 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
-      <c r="D25" s="44"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="42"/>
+      <c r="D25" s="35"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="19"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="42"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="19"/>
       <c r="B27" s="19"/>
       <c r="C27" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="G27" s="42"/>
+        <v>54</v>
+      </c>
+      <c r="F27" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="33"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="19"/>
       <c r="B28" s="19"/>
       <c r="C28" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="40"/>
+        <v>52</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="31"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="19"/>
       <c r="B29" s="19"/>
       <c r="C29" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>35</v>
@@ -3063,7 +3097,7 @@
       <c r="A30" s="19"/>
       <c r="B30" s="19"/>
       <c r="C30" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>34</v>
@@ -3092,1020 +3126,940 @@
   <dimension ref="A1:T117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G11" sqref="D10:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" style="32" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="9" style="32" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="6" style="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.5546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="33" customWidth="1"/>
-    <col min="10" max="10" width="8.77734375" style="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.77734375" style="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" style="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="2.109375" style="31" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="31"/>
+    <col min="1" max="1" width="7.90625" style="26" customWidth="1"/>
+    <col min="2" max="2" width="5.6328125" style="26" customWidth="1"/>
+    <col min="3" max="3" width="9" style="26" customWidth="1"/>
+    <col min="4" max="4" width="10" style="99" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" style="98" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="6" style="100" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.54296875" style="104" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6328125" style="102" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" style="98" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.81640625" style="88" customWidth="1"/>
+    <col min="13" max="13" width="6" style="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.26953125" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10" style="23" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.90625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="21"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="23">
+    <row r="1" spans="1:17" s="97" customFormat="1">
+      <c r="A1" s="89"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="91">
         <v>921</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="92" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="F1" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="H1" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="27">
-        <f>COUNT(H2:H500)</f>
+      <c r="I1" s="22">
+        <f>COUNT(I2:I500)</f>
         <v>0</v>
       </c>
-      <c r="I1" s="28">
-        <f>SUM(I2:I500)</f>
+      <c r="J1" s="87">
+        <f>SUM(J2:J500)</f>
         <v>0</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="K1" s="95" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" s="96" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="N1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="O1" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="C2" s="27"/>
+      <c r="D2" s="98"/>
+      <c r="J2" s="101"/>
+      <c r="O2" s="23" t="str">
+        <f>IF(ISNA(VLOOKUP(G2,A:B,2,0)),"",VLOOKUP(G2,A:B,2,0))</f>
+        <v/>
+      </c>
+      <c r="P2" s="103"/>
+      <c r="Q2" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="J3" s="101"/>
+      <c r="O3" s="23" t="str">
+        <f t="shared" ref="O3:O66" si="0">IF(ISNA(VLOOKUP(G3,A:B,2,0)),"",VLOOKUP(G3,A:B,2,0))</f>
+        <v/>
+      </c>
+      <c r="P3" s="103"/>
+      <c r="Q3" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="30" t="s">
+    </row>
+    <row r="4" spans="1:17">
+      <c r="J4" s="101"/>
+      <c r="O4" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P4" s="103"/>
+      <c r="Q4" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="C2" s="33"/>
-      <c r="I2" s="34"/>
-      <c r="K2" s="35"/>
-      <c r="M2" s="36" t="str">
-        <f>IF(ISNA(VLOOKUP(F2,A:B,2,0)),"",VLOOKUP(F2,A:B,2,0))</f>
-        <v/>
-      </c>
-      <c r="N2" s="37"/>
-      <c r="O2" s="36"/>
-      <c r="Q2" s="31" t="s">
+    </row>
+    <row r="5" spans="1:17">
+      <c r="J5" s="101"/>
+      <c r="O5" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
-      <c r="I3" s="34"/>
-      <c r="K3" s="35"/>
-      <c r="M3" s="36" t="str">
-        <f t="shared" ref="M3:M66" si="0">IF(ISNA(VLOOKUP(F3,A:B,2,0)),"",VLOOKUP(F3,A:B,2,0))</f>
-        <v/>
-      </c>
-      <c r="N3" s="37"/>
-      <c r="O3" s="36"/>
-      <c r="Q3" s="31" t="s">
+    <row r="6" spans="1:17">
+      <c r="J6" s="101"/>
+      <c r="O6" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
-      <c r="I4" s="34"/>
-      <c r="K4" s="35"/>
-      <c r="M4" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N4" s="37"/>
-      <c r="O4" s="36"/>
-      <c r="Q4" s="31" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="I5" s="34"/>
-      <c r="K5" s="35"/>
-      <c r="M5" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N5" s="37"/>
-      <c r="Q5" s="31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="I6" s="34"/>
-      <c r="K6" s="35"/>
-      <c r="M6" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N6" s="37"/>
-      <c r="Q6" s="31" t="s">
-        <v>51</v>
-      </c>
-    </row>
     <row r="7" spans="1:17">
-      <c r="I7" s="34"/>
-      <c r="K7" s="35"/>
-      <c r="M7" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N7" s="37"/>
-      <c r="O7" s="36"/>
+      <c r="J7" s="101"/>
+      <c r="O7" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P7" s="103"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="I8" s="34"/>
-      <c r="K8" s="35"/>
-      <c r="M8" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N8" s="37"/>
-      <c r="O8" s="36"/>
+      <c r="J8" s="101"/>
+      <c r="O8" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P8" s="103"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="I9" s="34"/>
-      <c r="K9" s="35"/>
-      <c r="M9" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N9" s="37"/>
-      <c r="O9" s="36"/>
+      <c r="J9" s="101"/>
+      <c r="O9" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P9" s="103"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="I10" s="34"/>
-      <c r="K10" s="35"/>
-      <c r="M10" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N10" s="37"/>
+      <c r="J10" s="101"/>
+      <c r="O10" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P10" s="103"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="I11" s="34"/>
-      <c r="K11" s="35"/>
-      <c r="M11" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N11" s="37"/>
+      <c r="J11" s="101"/>
+      <c r="O11" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P11" s="103"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="I12" s="34"/>
-      <c r="K12" s="35"/>
-      <c r="M12" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N12" s="37"/>
-      <c r="O12" s="36"/>
+      <c r="J12" s="101"/>
+      <c r="O12" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P12" s="103"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="I13" s="34"/>
-      <c r="K13" s="35"/>
-      <c r="M13" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N13" s="37"/>
-      <c r="O13" s="36"/>
+      <c r="J13" s="101"/>
+      <c r="O13" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P13" s="103"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="I14" s="34"/>
-      <c r="K14" s="35"/>
-      <c r="M14" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N14" s="37"/>
-      <c r="O14" s="36"/>
+      <c r="J14" s="101"/>
+      <c r="O14" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P14" s="103"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="I15" s="34"/>
-      <c r="K15" s="35"/>
-      <c r="M15" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N15" s="37"/>
+      <c r="J15" s="101"/>
+      <c r="O15" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P15" s="103"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="I16" s="34"/>
-      <c r="K16" s="35"/>
-      <c r="M16" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N16" s="37"/>
-    </row>
-    <row r="17" spans="9:15">
-      <c r="I17" s="34"/>
-      <c r="K17" s="35"/>
-      <c r="M17" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N17" s="37"/>
-      <c r="O17" s="36"/>
-    </row>
-    <row r="18" spans="9:15">
-      <c r="I18" s="34"/>
-      <c r="K18" s="35"/>
-      <c r="M18" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N18" s="37"/>
-      <c r="O18" s="36"/>
-    </row>
-    <row r="19" spans="9:15">
-      <c r="I19" s="34"/>
-      <c r="K19" s="35"/>
-      <c r="M19" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N19" s="37"/>
-      <c r="O19" s="36"/>
-    </row>
-    <row r="20" spans="9:15">
-      <c r="I20" s="34"/>
-      <c r="K20" s="35"/>
-      <c r="M20" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N20" s="37"/>
-    </row>
-    <row r="21" spans="9:15">
-      <c r="I21" s="34"/>
-      <c r="K21" s="35"/>
-      <c r="M21" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N21" s="37"/>
-    </row>
-    <row r="22" spans="9:15">
-      <c r="I22" s="34"/>
-      <c r="K22" s="35"/>
-      <c r="M22" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N22" s="37"/>
-      <c r="O22" s="36"/>
-    </row>
-    <row r="23" spans="9:15">
-      <c r="I23" s="34"/>
-      <c r="K23" s="35"/>
-      <c r="M23" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N23" s="37"/>
-      <c r="O23" s="36"/>
-    </row>
-    <row r="24" spans="9:15">
-      <c r="I24" s="34"/>
-      <c r="K24" s="35"/>
-      <c r="M24" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N24" s="37"/>
-      <c r="O24" s="36"/>
-    </row>
-    <row r="25" spans="9:15">
-      <c r="I25" s="34"/>
-      <c r="K25" s="35"/>
-      <c r="M25" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N25" s="37"/>
-    </row>
-    <row r="26" spans="9:15">
-      <c r="I26" s="34"/>
-      <c r="K26" s="35"/>
-      <c r="M26" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N26" s="37"/>
-    </row>
-    <row r="27" spans="9:15">
-      <c r="I27" s="34"/>
-      <c r="K27" s="35"/>
-      <c r="M27" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N27" s="37"/>
-      <c r="O27" s="36"/>
-    </row>
-    <row r="28" spans="9:15">
-      <c r="I28" s="34"/>
-      <c r="K28" s="35"/>
-      <c r="M28" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N28" s="37"/>
-      <c r="O28" s="36"/>
-    </row>
-    <row r="29" spans="9:15">
-      <c r="I29" s="34"/>
-      <c r="K29" s="35"/>
-      <c r="M29" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N29" s="37"/>
-      <c r="O29" s="36"/>
-    </row>
-    <row r="30" spans="9:15">
-      <c r="I30" s="34"/>
-      <c r="K30" s="35"/>
-      <c r="M30" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N30" s="37"/>
-    </row>
-    <row r="31" spans="9:15">
-      <c r="I31" s="34"/>
-      <c r="K31" s="35"/>
-      <c r="M31" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N31" s="37"/>
-    </row>
-    <row r="32" spans="9:15">
-      <c r="I32" s="34"/>
-      <c r="K32" s="35"/>
-      <c r="M32" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N32" s="37"/>
-      <c r="O32" s="36"/>
-    </row>
-    <row r="33" spans="9:20">
-      <c r="I33" s="34"/>
-      <c r="K33" s="35"/>
-      <c r="M33" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N33" s="37"/>
-      <c r="O33" s="36"/>
-    </row>
-    <row r="34" spans="9:20">
-      <c r="I34" s="34"/>
-      <c r="K34" s="35"/>
-      <c r="M34" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N34" s="37"/>
-      <c r="O34" s="36"/>
-    </row>
-    <row r="35" spans="9:20">
-      <c r="I35" s="34"/>
-      <c r="K35" s="35"/>
-      <c r="M35" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N35" s="37"/>
-    </row>
-    <row r="36" spans="9:20">
-      <c r="I36" s="34"/>
-      <c r="K36" s="35"/>
-      <c r="M36" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N36" s="37"/>
-    </row>
-    <row r="37" spans="9:20">
-      <c r="I37" s="34"/>
-      <c r="K37" s="35"/>
-      <c r="M37" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N37" s="37"/>
-    </row>
-    <row r="38" spans="9:20">
-      <c r="I38" s="34"/>
-      <c r="K38" s="35"/>
-      <c r="M38" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N38" s="37"/>
-    </row>
-    <row r="39" spans="9:20">
-      <c r="I39" s="34"/>
-      <c r="K39" s="35"/>
-      <c r="M39" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N39" s="37"/>
-    </row>
-    <row r="40" spans="9:20">
-      <c r="I40" s="34"/>
-      <c r="K40" s="35"/>
-      <c r="M40" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N40" s="37"/>
-    </row>
-    <row r="41" spans="9:20">
-      <c r="I41" s="34"/>
-      <c r="K41" s="35"/>
-      <c r="M41" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N41" s="37"/>
-    </row>
-    <row r="42" spans="9:20">
-      <c r="I42" s="34"/>
-      <c r="K42" s="35"/>
-      <c r="M42" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N42" s="37"/>
-    </row>
-    <row r="43" spans="9:20">
-      <c r="I43" s="34"/>
-      <c r="K43" s="35"/>
-      <c r="M43" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N43" s="37"/>
-    </row>
-    <row r="44" spans="9:20">
-      <c r="I44" s="34"/>
-      <c r="K44" s="35"/>
-      <c r="M44" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N44" s="37"/>
-    </row>
-    <row r="45" spans="9:20">
-      <c r="I45" s="34"/>
-      <c r="K45" s="35"/>
-      <c r="M45" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N45" s="37"/>
-    </row>
-    <row r="46" spans="9:20">
-      <c r="I46" s="34"/>
-      <c r="K46" s="35"/>
-      <c r="M46" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N46" s="37"/>
-    </row>
-    <row r="47" spans="9:20">
-      <c r="I47" s="34"/>
-      <c r="K47" s="38"/>
-      <c r="M47" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N47" s="37"/>
-      <c r="P47" s="39"/>
-      <c r="Q47" s="39"/>
-      <c r="R47" s="39"/>
-      <c r="S47" s="39"/>
-      <c r="T47" s="39"/>
-    </row>
-    <row r="48" spans="9:20">
-      <c r="I48" s="34"/>
-      <c r="K48" s="35"/>
-      <c r="M48" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N48" s="37"/>
-    </row>
-    <row r="49" spans="9:14">
-      <c r="I49" s="34"/>
-      <c r="K49" s="35"/>
-      <c r="M49" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N49" s="37"/>
-    </row>
-    <row r="50" spans="9:14">
-      <c r="K50" s="35"/>
-      <c r="M50" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N50" s="37"/>
-    </row>
-    <row r="51" spans="9:14">
-      <c r="K51" s="35"/>
-      <c r="M51" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N51" s="37"/>
-    </row>
-    <row r="52" spans="9:14">
-      <c r="K52" s="35"/>
-      <c r="M52" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N52" s="37"/>
-    </row>
-    <row r="53" spans="9:14">
-      <c r="K53" s="35"/>
-      <c r="M53" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N53" s="37"/>
-    </row>
-    <row r="54" spans="9:14">
-      <c r="K54" s="35"/>
-      <c r="M54" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N54" s="37"/>
-    </row>
-    <row r="55" spans="9:14">
-      <c r="K55" s="35"/>
-      <c r="M55" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N55" s="37"/>
-    </row>
-    <row r="56" spans="9:14">
-      <c r="K56" s="35"/>
-      <c r="M56" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N56" s="37"/>
-    </row>
-    <row r="57" spans="9:14">
-      <c r="K57" s="35"/>
-      <c r="M57" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N57" s="37"/>
-    </row>
-    <row r="58" spans="9:14">
-      <c r="K58" s="35"/>
-      <c r="M58" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N58" s="37"/>
-    </row>
-    <row r="59" spans="9:14">
-      <c r="K59" s="35"/>
-      <c r="M59" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N59" s="37"/>
-    </row>
-    <row r="60" spans="9:14">
-      <c r="K60" s="35"/>
-      <c r="M60" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N60" s="37"/>
-    </row>
-    <row r="61" spans="9:14">
-      <c r="K61" s="35"/>
-      <c r="M61" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N61" s="37"/>
-    </row>
-    <row r="62" spans="9:14">
-      <c r="K62" s="35"/>
-      <c r="M62" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N62" s="37"/>
-    </row>
-    <row r="63" spans="9:14">
-      <c r="K63" s="35"/>
-      <c r="M63" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N63" s="37"/>
-    </row>
-    <row r="64" spans="9:14">
-      <c r="K64" s="35"/>
-      <c r="M64" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N64" s="37"/>
-    </row>
-    <row r="65" spans="11:14">
-      <c r="K65" s="35"/>
-      <c r="M65" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N65" s="37"/>
-    </row>
-    <row r="66" spans="11:14">
-      <c r="K66" s="35"/>
-      <c r="M66" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N66" s="37"/>
-    </row>
-    <row r="67" spans="11:14">
-      <c r="K67" s="35"/>
-      <c r="M67" s="36" t="str">
-        <f t="shared" ref="M67:M113" si="1">IF(ISNA(VLOOKUP(F67,A:B,2,0)),"",VLOOKUP(F67,A:B,2,0))</f>
-        <v/>
-      </c>
-      <c r="N67" s="37"/>
-    </row>
-    <row r="68" spans="11:14">
-      <c r="M68" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N68" s="37"/>
-    </row>
-    <row r="69" spans="11:14">
-      <c r="M69" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N69" s="37"/>
-    </row>
-    <row r="70" spans="11:14">
-      <c r="M70" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N70" s="37"/>
-    </row>
-    <row r="71" spans="11:14">
-      <c r="M71" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N71" s="37"/>
-    </row>
-    <row r="72" spans="11:14">
-      <c r="M72" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N72" s="37"/>
-    </row>
-    <row r="73" spans="11:14">
-      <c r="M73" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N73" s="37"/>
-    </row>
-    <row r="74" spans="11:14">
-      <c r="M74" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N74" s="37"/>
-    </row>
-    <row r="75" spans="11:14">
-      <c r="M75" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N75" s="37"/>
-    </row>
-    <row r="76" spans="11:14">
-      <c r="M76" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N76" s="37"/>
-    </row>
-    <row r="77" spans="11:14">
-      <c r="M77" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N77" s="37"/>
-    </row>
-    <row r="78" spans="11:14">
-      <c r="M78" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N78" s="37"/>
-    </row>
-    <row r="79" spans="11:14">
-      <c r="M79" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N79" s="37"/>
-    </row>
-    <row r="80" spans="11:14">
-      <c r="M80" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N80" s="37"/>
-    </row>
-    <row r="81" spans="13:14">
-      <c r="M81" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N81" s="37"/>
-    </row>
-    <row r="82" spans="13:14">
-      <c r="M82" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N82" s="37"/>
-    </row>
-    <row r="83" spans="13:14">
-      <c r="M83" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N83" s="37"/>
-    </row>
-    <row r="84" spans="13:14">
-      <c r="M84" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N84" s="37"/>
-    </row>
-    <row r="85" spans="13:14">
-      <c r="M85" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N85" s="37"/>
-    </row>
-    <row r="86" spans="13:14">
-      <c r="M86" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N86" s="37"/>
-    </row>
-    <row r="87" spans="13:14">
-      <c r="M87" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N87" s="37"/>
-    </row>
-    <row r="88" spans="13:14">
-      <c r="M88" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N88" s="37"/>
-    </row>
-    <row r="89" spans="13:14">
-      <c r="M89" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N89" s="37"/>
-    </row>
-    <row r="90" spans="13:14">
-      <c r="M90" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N90" s="37"/>
-    </row>
-    <row r="91" spans="13:14">
-      <c r="M91" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N91" s="37"/>
-    </row>
-    <row r="92" spans="13:14">
-      <c r="M92" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N92" s="37"/>
-    </row>
-    <row r="93" spans="13:14">
-      <c r="M93" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N93" s="37"/>
-    </row>
-    <row r="94" spans="13:14">
-      <c r="M94" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N94" s="37"/>
-    </row>
-    <row r="95" spans="13:14">
-      <c r="M95" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N95" s="37"/>
-    </row>
-    <row r="96" spans="13:14">
-      <c r="M96" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N96" s="37"/>
-    </row>
-    <row r="97" spans="13:14">
-      <c r="M97" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N97" s="37"/>
-    </row>
-    <row r="98" spans="13:14">
-      <c r="M98" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N98" s="37"/>
-    </row>
-    <row r="99" spans="13:14">
-      <c r="M99" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N99" s="37"/>
-    </row>
-    <row r="100" spans="13:14">
-      <c r="M100" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N100" s="37"/>
-    </row>
-    <row r="101" spans="13:14">
-      <c r="M101" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N101" s="37"/>
-    </row>
-    <row r="102" spans="13:14">
-      <c r="M102" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N102" s="37"/>
-    </row>
-    <row r="103" spans="13:14">
-      <c r="M103" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N103" s="37"/>
-    </row>
-    <row r="104" spans="13:14">
-      <c r="M104" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N104" s="37"/>
-    </row>
-    <row r="105" spans="13:14">
-      <c r="M105" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N105" s="37"/>
-    </row>
-    <row r="106" spans="13:14">
-      <c r="M106" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N106" s="37"/>
-    </row>
-    <row r="107" spans="13:14">
-      <c r="M107" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N107" s="37"/>
-    </row>
-    <row r="108" spans="13:14">
-      <c r="M108" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N108" s="37"/>
-    </row>
-    <row r="109" spans="13:14">
-      <c r="M109" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N109" s="37"/>
-    </row>
-    <row r="110" spans="13:14">
-      <c r="M110" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N110" s="37"/>
-    </row>
-    <row r="111" spans="13:14">
-      <c r="M111" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N111" s="37"/>
-    </row>
-    <row r="112" spans="13:14">
-      <c r="M112" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N112" s="37"/>
-    </row>
-    <row r="113" spans="13:14">
-      <c r="M113" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N113" s="37"/>
-    </row>
-    <row r="114" spans="13:14">
-      <c r="N114" s="37"/>
-    </row>
-    <row r="115" spans="13:14">
-      <c r="N115" s="37"/>
-    </row>
-    <row r="116" spans="13:14">
-      <c r="N116" s="37"/>
-    </row>
-    <row r="117" spans="13:14">
-      <c r="N117" s="37"/>
+      <c r="J16" s="101"/>
+      <c r="O16" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P16" s="103"/>
+    </row>
+    <row r="17" spans="10:16">
+      <c r="J17" s="101"/>
+      <c r="O17" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P17" s="103"/>
+    </row>
+    <row r="18" spans="10:16">
+      <c r="J18" s="101"/>
+      <c r="O18" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P18" s="103"/>
+    </row>
+    <row r="19" spans="10:16">
+      <c r="J19" s="101"/>
+      <c r="O19" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P19" s="103"/>
+    </row>
+    <row r="20" spans="10:16">
+      <c r="J20" s="101"/>
+      <c r="O20" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P20" s="103"/>
+    </row>
+    <row r="21" spans="10:16">
+      <c r="J21" s="101"/>
+      <c r="O21" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P21" s="103"/>
+    </row>
+    <row r="22" spans="10:16">
+      <c r="J22" s="101"/>
+      <c r="O22" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P22" s="103"/>
+    </row>
+    <row r="23" spans="10:16">
+      <c r="J23" s="101"/>
+      <c r="O23" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P23" s="103"/>
+    </row>
+    <row r="24" spans="10:16">
+      <c r="J24" s="101"/>
+      <c r="O24" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P24" s="103"/>
+    </row>
+    <row r="25" spans="10:16">
+      <c r="J25" s="101"/>
+      <c r="O25" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P25" s="103"/>
+    </row>
+    <row r="26" spans="10:16">
+      <c r="J26" s="101"/>
+      <c r="O26" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P26" s="103"/>
+    </row>
+    <row r="27" spans="10:16">
+      <c r="J27" s="101"/>
+      <c r="O27" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P27" s="103"/>
+    </row>
+    <row r="28" spans="10:16">
+      <c r="J28" s="101"/>
+      <c r="O28" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P28" s="103"/>
+    </row>
+    <row r="29" spans="10:16">
+      <c r="J29" s="101"/>
+      <c r="O29" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P29" s="103"/>
+    </row>
+    <row r="30" spans="10:16">
+      <c r="J30" s="101"/>
+      <c r="O30" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P30" s="103"/>
+    </row>
+    <row r="31" spans="10:16">
+      <c r="J31" s="101"/>
+      <c r="O31" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P31" s="103"/>
+    </row>
+    <row r="32" spans="10:16">
+      <c r="J32" s="101"/>
+      <c r="O32" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P32" s="103"/>
+    </row>
+    <row r="33" spans="10:20">
+      <c r="J33" s="101"/>
+      <c r="O33" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P33" s="103"/>
+    </row>
+    <row r="34" spans="10:20">
+      <c r="J34" s="101"/>
+      <c r="O34" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P34" s="103"/>
+    </row>
+    <row r="35" spans="10:20">
+      <c r="J35" s="101"/>
+      <c r="O35" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P35" s="103"/>
+    </row>
+    <row r="36" spans="10:20">
+      <c r="J36" s="101"/>
+      <c r="O36" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P36" s="103"/>
+    </row>
+    <row r="37" spans="10:20">
+      <c r="J37" s="101"/>
+      <c r="O37" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P37" s="103"/>
+    </row>
+    <row r="38" spans="10:20">
+      <c r="J38" s="101"/>
+      <c r="O38" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P38" s="103"/>
+    </row>
+    <row r="39" spans="10:20">
+      <c r="J39" s="101"/>
+      <c r="O39" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P39" s="103"/>
+    </row>
+    <row r="40" spans="10:20">
+      <c r="J40" s="101"/>
+      <c r="O40" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P40" s="103"/>
+    </row>
+    <row r="41" spans="10:20">
+      <c r="J41" s="101"/>
+      <c r="O41" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P41" s="103"/>
+    </row>
+    <row r="42" spans="10:20">
+      <c r="J42" s="101"/>
+      <c r="O42" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P42" s="103"/>
+    </row>
+    <row r="43" spans="10:20">
+      <c r="J43" s="101"/>
+      <c r="O43" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P43" s="103"/>
+    </row>
+    <row r="44" spans="10:20">
+      <c r="J44" s="101"/>
+      <c r="O44" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P44" s="103"/>
+    </row>
+    <row r="45" spans="10:20">
+      <c r="J45" s="101"/>
+      <c r="O45" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P45" s="103"/>
+    </row>
+    <row r="46" spans="10:20">
+      <c r="J46" s="101"/>
+      <c r="O46" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P46" s="103"/>
+    </row>
+    <row r="47" spans="10:20">
+      <c r="J47" s="101"/>
+      <c r="M47" s="29"/>
+      <c r="O47" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P47" s="103"/>
+      <c r="Q47" s="30"/>
+      <c r="R47" s="30"/>
+      <c r="S47" s="30"/>
+      <c r="T47" s="30"/>
+    </row>
+    <row r="48" spans="10:20">
+      <c r="J48" s="101"/>
+      <c r="O48" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P48" s="103"/>
+    </row>
+    <row r="49" spans="10:16">
+      <c r="J49" s="101"/>
+      <c r="O49" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P49" s="103"/>
+    </row>
+    <row r="50" spans="10:16">
+      <c r="O50" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P50" s="103"/>
+    </row>
+    <row r="51" spans="10:16">
+      <c r="O51" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P51" s="103"/>
+    </row>
+    <row r="52" spans="10:16">
+      <c r="O52" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P52" s="103"/>
+    </row>
+    <row r="53" spans="10:16">
+      <c r="O53" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P53" s="103"/>
+    </row>
+    <row r="54" spans="10:16">
+      <c r="O54" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P54" s="103"/>
+    </row>
+    <row r="55" spans="10:16">
+      <c r="O55" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P55" s="103"/>
+    </row>
+    <row r="56" spans="10:16">
+      <c r="O56" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P56" s="103"/>
+    </row>
+    <row r="57" spans="10:16">
+      <c r="O57" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P57" s="103"/>
+    </row>
+    <row r="58" spans="10:16">
+      <c r="O58" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P58" s="103"/>
+    </row>
+    <row r="59" spans="10:16">
+      <c r="O59" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P59" s="103"/>
+    </row>
+    <row r="60" spans="10:16">
+      <c r="O60" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P60" s="103"/>
+    </row>
+    <row r="61" spans="10:16">
+      <c r="O61" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P61" s="103"/>
+    </row>
+    <row r="62" spans="10:16">
+      <c r="O62" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P62" s="103"/>
+    </row>
+    <row r="63" spans="10:16">
+      <c r="O63" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P63" s="103"/>
+    </row>
+    <row r="64" spans="10:16">
+      <c r="O64" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P64" s="103"/>
+    </row>
+    <row r="65" spans="15:16">
+      <c r="O65" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P65" s="103"/>
+    </row>
+    <row r="66" spans="15:16">
+      <c r="O66" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P66" s="103"/>
+    </row>
+    <row r="67" spans="15:16">
+      <c r="O67" s="23" t="str">
+        <f t="shared" ref="O67:O113" si="1">IF(ISNA(VLOOKUP(G67,A:B,2,0)),"",VLOOKUP(G67,A:B,2,0))</f>
+        <v/>
+      </c>
+      <c r="P67" s="103"/>
+    </row>
+    <row r="68" spans="15:16">
+      <c r="O68" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P68" s="103"/>
+    </row>
+    <row r="69" spans="15:16">
+      <c r="O69" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P69" s="103"/>
+    </row>
+    <row r="70" spans="15:16">
+      <c r="O70" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P70" s="103"/>
+    </row>
+    <row r="71" spans="15:16">
+      <c r="O71" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P71" s="103"/>
+    </row>
+    <row r="72" spans="15:16">
+      <c r="O72" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P72" s="103"/>
+    </row>
+    <row r="73" spans="15:16">
+      <c r="O73" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P73" s="103"/>
+    </row>
+    <row r="74" spans="15:16">
+      <c r="O74" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P74" s="103"/>
+    </row>
+    <row r="75" spans="15:16">
+      <c r="O75" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P75" s="103"/>
+    </row>
+    <row r="76" spans="15:16">
+      <c r="O76" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P76" s="103"/>
+    </row>
+    <row r="77" spans="15:16">
+      <c r="O77" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P77" s="103"/>
+    </row>
+    <row r="78" spans="15:16">
+      <c r="O78" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P78" s="103"/>
+    </row>
+    <row r="79" spans="15:16">
+      <c r="O79" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P79" s="103"/>
+    </row>
+    <row r="80" spans="15:16">
+      <c r="O80" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P80" s="103"/>
+    </row>
+    <row r="81" spans="15:16">
+      <c r="O81" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P81" s="103"/>
+    </row>
+    <row r="82" spans="15:16">
+      <c r="O82" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P82" s="103"/>
+    </row>
+    <row r="83" spans="15:16">
+      <c r="O83" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P83" s="103"/>
+    </row>
+    <row r="84" spans="15:16">
+      <c r="O84" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P84" s="103"/>
+    </row>
+    <row r="85" spans="15:16">
+      <c r="O85" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P85" s="103"/>
+    </row>
+    <row r="86" spans="15:16">
+      <c r="O86" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P86" s="103"/>
+    </row>
+    <row r="87" spans="15:16">
+      <c r="O87" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P87" s="103"/>
+    </row>
+    <row r="88" spans="15:16">
+      <c r="O88" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P88" s="103"/>
+    </row>
+    <row r="89" spans="15:16">
+      <c r="O89" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P89" s="103"/>
+    </row>
+    <row r="90" spans="15:16">
+      <c r="O90" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P90" s="103"/>
+    </row>
+    <row r="91" spans="15:16">
+      <c r="O91" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P91" s="103"/>
+    </row>
+    <row r="92" spans="15:16">
+      <c r="O92" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P92" s="103"/>
+    </row>
+    <row r="93" spans="15:16">
+      <c r="O93" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P93" s="103"/>
+    </row>
+    <row r="94" spans="15:16">
+      <c r="O94" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P94" s="103"/>
+    </row>
+    <row r="95" spans="15:16">
+      <c r="O95" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P95" s="103"/>
+    </row>
+    <row r="96" spans="15:16">
+      <c r="O96" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P96" s="103"/>
+    </row>
+    <row r="97" spans="15:16">
+      <c r="O97" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P97" s="103"/>
+    </row>
+    <row r="98" spans="15:16">
+      <c r="O98" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P98" s="103"/>
+    </row>
+    <row r="99" spans="15:16">
+      <c r="O99" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P99" s="103"/>
+    </row>
+    <row r="100" spans="15:16">
+      <c r="O100" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P100" s="103"/>
+    </row>
+    <row r="101" spans="15:16">
+      <c r="O101" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P101" s="103"/>
+    </row>
+    <row r="102" spans="15:16">
+      <c r="O102" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P102" s="103"/>
+    </row>
+    <row r="103" spans="15:16">
+      <c r="O103" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P103" s="103"/>
+    </row>
+    <row r="104" spans="15:16">
+      <c r="O104" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P104" s="103"/>
+    </row>
+    <row r="105" spans="15:16">
+      <c r="O105" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P105" s="103"/>
+    </row>
+    <row r="106" spans="15:16">
+      <c r="O106" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P106" s="103"/>
+    </row>
+    <row r="107" spans="15:16">
+      <c r="O107" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P107" s="103"/>
+    </row>
+    <row r="108" spans="15:16">
+      <c r="O108" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P108" s="103"/>
+    </row>
+    <row r="109" spans="15:16">
+      <c r="O109" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P109" s="103"/>
+    </row>
+    <row r="110" spans="15:16">
+      <c r="O110" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P110" s="103"/>
+    </row>
+    <row r="111" spans="15:16">
+      <c r="O111" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P111" s="103"/>
+    </row>
+    <row r="112" spans="15:16">
+      <c r="O112" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P112" s="103"/>
+    </row>
+    <row r="113" spans="15:16">
+      <c r="O113" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P113" s="103"/>
+    </row>
+    <row r="114" spans="15:16">
+      <c r="P114" s="103"/>
+    </row>
+    <row r="115" spans="15:16">
+      <c r="P115" s="103"/>
+    </row>
+    <row r="116" spans="15:16">
+      <c r="P116" s="103"/>
+    </row>
+    <row r="117" spans="15:16">
+      <c r="P117" s="103"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Auto-committed on 2022/05/20 週五 11:31:56.86
</commit_message>
<xml_diff>
--- a/Program/Other/LM057_底稿_表14-5、14-6_會計部申報表.xlsx
+++ b/Program/Other/LM057_底稿_表14-5、14-6_會計部申報表.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5950" yWindow="120" windowWidth="6000" windowHeight="6410" tabRatio="853" activeTab="2"/>
+    <workbookView xWindow="5950" yWindow="120" windowWidth="6000" windowHeight="6410" tabRatio="853" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="表14-6" sheetId="4" r:id="rId1"/>
@@ -1253,11 +1253,11 @@
     <numFmt numFmtId="176" formatCode="#,##0_ "/>
     <numFmt numFmtId="177" formatCode="0.000%"/>
     <numFmt numFmtId="178" formatCode="#,##0_);[Red]\(#,##0\)"/>
-    <numFmt numFmtId="180" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="181" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="182" formatCode="0.000_ "/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="181" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -1758,7 +1758,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="9" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1785,7 +1785,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="14" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="14" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1794,7 +1794,7 @@
     <xf numFmtId="41" fontId="14" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="18" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="18" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1803,7 +1803,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="14" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="179" fontId="14" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1821,16 +1821,16 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1854,11 +1854,65 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="14" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1913,60 +1967,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="14" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="1" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="0" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2345,7 +2345,7 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="5" style="4" customWidth="1"/>
     <col min="2" max="2" width="15.1796875" style="4" customWidth="1"/>
@@ -2354,7 +2354,7 @@
     <col min="5" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5">
+    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A1" s="7"/>
       <c r="B1" s="15" t="s">
         <v>36</v>
@@ -2364,7 +2364,7 @@
       </c>
       <c r="D1" s="13"/>
     </row>
-    <row r="2" spans="1:4" ht="19.5">
+    <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A2" s="7"/>
       <c r="B2" s="13"/>
       <c r="C2" s="10" t="s">
@@ -2375,7 +2375,7 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.5">
+    <row r="3" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
@@ -2385,23 +2385,23 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="19.5">
+    <row r="4" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="69"/>
+      <c r="C4" s="87"/>
       <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="19.5">
+    <row r="5" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="88" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2409,71 +2409,71 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="24" customHeight="1">
+    <row r="6" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="71"/>
+      <c r="B6" s="89"/>
       <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="19.5">
+    <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="71"/>
+      <c r="B7" s="89"/>
       <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="19.5">
+    <row r="8" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="71"/>
+      <c r="B8" s="89"/>
       <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="19.5">
+    <row r="9" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" s="71"/>
+      <c r="B9" s="89"/>
       <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="19.5">
+    <row r="10" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>6</v>
       </c>
-      <c r="B10" s="71"/>
+      <c r="B10" s="89"/>
       <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="19.5">
+    <row r="11" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>7</v>
       </c>
-      <c r="B11" s="71"/>
+      <c r="B11" s="89"/>
       <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="19.5">
+    <row r="12" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="91" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -2484,11 +2484,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="19.5">
+    <row r="13" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>9</v>
       </c>
-      <c r="B13" s="74"/>
+      <c r="B13" s="92"/>
       <c r="C13" s="12" t="s">
         <v>0</v>
       </c>
@@ -2497,11 +2497,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="19.5">
+    <row r="14" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>10</v>
       </c>
-      <c r="B14" s="75"/>
+      <c r="B14" s="93"/>
       <c r="C14" s="12" t="s">
         <v>1</v>
       </c>
@@ -2510,60 +2510,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="19.5">
+    <row r="15" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>11</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="72"/>
+      <c r="C15" s="90"/>
       <c r="D15" s="17">
         <f>'14-5申報表'!D18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="19.5">
+    <row r="16" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>12</v>
       </c>
-      <c r="B16" s="76" t="s">
+      <c r="B16" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="77"/>
+      <c r="C16" s="95"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="39" customHeight="1">
+    <row r="17" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>13</v>
       </c>
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="79"/>
+      <c r="C17" s="97"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="39" customHeight="1">
+    <row r="18" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>14</v>
       </c>
-      <c r="B18" s="78" t="s">
+      <c r="B18" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="79"/>
+      <c r="C18" s="97"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="19.5">
+    <row r="19" spans="1:5" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>15</v>
       </c>
-      <c r="B19" s="76" t="s">
+      <c r="B19" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="77"/>
+      <c r="C19" s="95"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="19.5">
+    <row r="20" spans="1:5" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="19.5">
+    <row r="21" spans="1:5" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -2586,27 +2586,27 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:5" ht="39.75" customHeight="1">
+    <row r="22" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>18</v>
       </c>
-      <c r="B22" s="70" t="s">
+      <c r="B22" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="70"/>
+      <c r="C22" s="88"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:5" ht="36" customHeight="1">
+    <row r="23" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>19</v>
       </c>
-      <c r="B23" s="70" t="s">
+      <c r="B23" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="70"/>
+      <c r="C23" s="88"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:5" ht="19.5">
+    <row r="24" spans="1:5" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -2616,7 +2616,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="11" t="s">
         <v>10</v>
       </c>
@@ -2625,14 +2625,14 @@
       <c r="D25" s="11"/>
       <c r="E25" s="14"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="14"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C27" s="8" t="s">
         <v>32</v>
       </c>
@@ -2640,12 +2640,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C28" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C29" s="8" t="s">
         <v>12</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C30" s="8" t="s">
         <v>26</v>
       </c>
@@ -2691,11 +2691,11 @@
   </sheetPr>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.81640625" customWidth="1"/>
     <col min="2" max="2" width="10.453125" customWidth="1"/>
@@ -2707,7 +2707,7 @@
     <col min="8" max="8" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5">
+    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A1" s="66"/>
       <c r="B1" s="15" t="s">
         <v>87</v>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="D1" s="65"/>
     </row>
-    <row r="2" spans="1:7" ht="17.5">
+    <row r="2" spans="1:7" ht="17.5" x14ac:dyDescent="0.4">
       <c r="A2" s="66"/>
       <c r="B2" s="65"/>
       <c r="C2" s="10" t="s">
@@ -2727,7 +2727,7 @@
         <v>43585</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>85</v>
       </c>
@@ -2737,23 +2737,23 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="83"/>
+      <c r="C4" s="101"/>
       <c r="D4" s="63" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="34">
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.4">
       <c r="A5" s="43">
         <v>1</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="102" t="s">
         <v>82</v>
       </c>
       <c r="C5" s="52" t="s">
@@ -2763,11 +2763,11 @@
       <c r="F5" s="38"/>
       <c r="G5" s="39"/>
     </row>
-    <row r="6" spans="1:7" ht="34">
+    <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.4">
       <c r="A6" s="43">
         <v>2</v>
       </c>
-      <c r="B6" s="85"/>
+      <c r="B6" s="103"/>
       <c r="C6" s="52" t="s">
         <v>80</v>
       </c>
@@ -2779,11 +2779,11 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="26.4" customHeight="1">
+    <row r="7" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="43">
         <v>3</v>
       </c>
-      <c r="B7" s="85"/>
+      <c r="B7" s="103"/>
       <c r="C7" s="62" t="s">
         <v>78</v>
       </c>
@@ -2793,11 +2793,11 @@
       </c>
       <c r="G7" s="59"/>
     </row>
-    <row r="8" spans="1:7" ht="34">
+    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.4">
       <c r="A8" s="43">
         <v>4</v>
       </c>
-      <c r="B8" s="85"/>
+      <c r="B8" s="103"/>
       <c r="C8" s="57" t="s">
         <v>77</v>
       </c>
@@ -2807,11 +2807,11 @@
       </c>
       <c r="G8" s="67"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="43">
         <v>5</v>
       </c>
-      <c r="B9" s="85"/>
+      <c r="B9" s="103"/>
       <c r="C9" s="49" t="s">
         <v>76</v>
       </c>
@@ -2824,11 +2824,11 @@
       </c>
       <c r="G9" s="67"/>
     </row>
-    <row r="10" spans="1:7" ht="34">
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.4">
       <c r="A10" s="43">
         <v>6</v>
       </c>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="102" t="s">
         <v>75</v>
       </c>
       <c r="C10" s="57" t="s">
@@ -2840,11 +2840,11 @@
       </c>
       <c r="G10" s="59"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="43">
         <v>7</v>
       </c>
-      <c r="B11" s="86"/>
+      <c r="B11" s="104"/>
       <c r="C11" s="57" t="s">
         <v>73</v>
       </c>
@@ -2854,11 +2854,11 @@
       </c>
       <c r="G11" s="58"/>
     </row>
-    <row r="12" spans="1:7" ht="34">
+    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.4">
       <c r="A12" s="43">
         <v>8</v>
       </c>
-      <c r="B12" s="86"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="57" t="s">
         <v>72</v>
       </c>
@@ -2868,11 +2868,11 @@
       </c>
       <c r="G12" s="56"/>
     </row>
-    <row r="13" spans="1:7" ht="51">
+    <row r="13" spans="1:7" ht="51" x14ac:dyDescent="0.4">
       <c r="A13" s="43">
         <v>9</v>
       </c>
-      <c r="B13" s="86"/>
+      <c r="B13" s="104"/>
       <c r="C13" s="52" t="s">
         <v>71</v>
       </c>
@@ -2882,11 +2882,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="43">
         <v>10</v>
       </c>
-      <c r="B14" s="86"/>
+      <c r="B14" s="104"/>
       <c r="C14" s="52" t="s">
         <v>70</v>
       </c>
@@ -2896,11 +2896,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="34">
+    <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.4">
       <c r="A15" s="43">
         <v>11</v>
       </c>
-      <c r="B15" s="86"/>
+      <c r="B15" s="104"/>
       <c r="C15" s="52" t="s">
         <v>69</v>
       </c>
@@ -2912,11 +2912,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="43">
         <v>12</v>
       </c>
-      <c r="B16" s="86"/>
+      <c r="B16" s="104"/>
       <c r="C16" s="52" t="s">
         <v>67</v>
       </c>
@@ -2928,11 +2928,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" s="43">
         <v>13</v>
       </c>
-      <c r="B17" s="86"/>
+      <c r="B17" s="104"/>
       <c r="C17" s="49" t="s">
         <v>65</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" s="43">
         <v>14</v>
       </c>
@@ -2953,7 +2953,7 @@
       <c r="F18" s="47"/>
       <c r="G18" s="46"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" s="43">
         <v>15</v>
       </c>
@@ -2961,10 +2961,7 @@
         <v>63</v>
       </c>
       <c r="C19" s="42"/>
-      <c r="D19" s="45">
-        <f>D9+D17+G15+G16</f>
-        <v>0</v>
-      </c>
+      <c r="D19" s="45"/>
       <c r="F19" s="44">
         <v>0</v>
       </c>
@@ -2972,7 +2969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" s="43">
         <v>16</v>
       </c>
@@ -2985,7 +2982,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A21" s="43">
         <v>17</v>
       </c>
@@ -2998,7 +2995,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" s="43">
         <v>18</v>
       </c>
@@ -3013,7 +3010,7 @@
       <c r="F22" s="38"/>
       <c r="G22" s="39"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>59</v>
       </c>
@@ -3026,13 +3023,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="36" customFormat="1">
-      <c r="A24" s="80" t="s">
+    <row r="24" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="81"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="99"/>
       <c r="F24" s="38"/>
       <c r="G24" s="37"/>
       <c r="H24"/>
@@ -3041,7 +3038,7 @@
       <c r="K24"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>56</v>
       </c>
@@ -3051,14 +3048,14 @@
       <c r="F25" s="34"/>
       <c r="G25" s="33"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" s="19"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
       <c r="F26" s="34"/>
       <c r="G26" s="33"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" s="19"/>
       <c r="B27" s="19"/>
       <c r="C27" s="8" t="s">
@@ -3072,7 +3069,7 @@
       </c>
       <c r="G27" s="33"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" s="19"/>
       <c r="B28" s="19"/>
       <c r="C28" s="8" t="s">
@@ -3083,7 +3080,7 @@
       </c>
       <c r="G28" s="31"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A29" s="19"/>
       <c r="B29" s="19"/>
       <c r="C29" s="8" t="s">
@@ -3093,7 +3090,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A30" s="19"/>
       <c r="B30" s="19"/>
       <c r="C30" s="8" t="s">
@@ -3125,61 +3122,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="D10:G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="7.90625" style="26" customWidth="1"/>
     <col min="2" max="2" width="5.6328125" style="26" customWidth="1"/>
     <col min="3" max="3" width="9" style="26" customWidth="1"/>
-    <col min="4" max="4" width="10" style="99" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="98" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="6" style="100" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.54296875" style="104" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6328125" style="102" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" style="98" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.81640625" style="88" customWidth="1"/>
+    <col min="4" max="4" width="10" style="81" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" style="80" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="6" style="82" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.54296875" style="86" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6328125" style="84" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.81640625" style="70" customWidth="1"/>
     <col min="13" max="13" width="6" style="28" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.26953125" style="24" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" style="23" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="8.90625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="97" customFormat="1">
-      <c r="A1" s="89"/>
-      <c r="B1" s="90"/>
-      <c r="C1" s="91">
+    <row r="1" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="71"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="73">
         <v>921</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="94" t="s">
+      <c r="F1" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="94" t="s">
+      <c r="G1" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="94" t="s">
+      <c r="H1" s="76" t="s">
         <v>41</v>
       </c>
       <c r="I1" s="22">
         <f>COUNT(I2:I500)</f>
         <v>0</v>
       </c>
-      <c r="J1" s="87">
+      <c r="J1" s="69">
         <f>SUM(J2:J500)</f>
         <v>0</v>
       </c>
-      <c r="K1" s="95" t="s">
+      <c r="K1" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="96" t="s">
+      <c r="L1" s="78" t="s">
         <v>93</v>
       </c>
       <c r="M1" s="21" t="s">
@@ -3195,871 +3192,871 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="C2" s="27"/>
-      <c r="D2" s="98"/>
-      <c r="J2" s="101"/>
+      <c r="D2" s="80"/>
+      <c r="J2" s="83"/>
       <c r="O2" s="23" t="str">
         <f>IF(ISNA(VLOOKUP(G2,A:B,2,0)),"",VLOOKUP(G2,A:B,2,0))</f>
         <v/>
       </c>
-      <c r="P2" s="103"/>
+      <c r="P2" s="85"/>
       <c r="Q2" s="25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
-      <c r="J3" s="101"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="J3" s="83"/>
       <c r="O3" s="23" t="str">
         <f t="shared" ref="O3:O66" si="0">IF(ISNA(VLOOKUP(G3,A:B,2,0)),"",VLOOKUP(G3,A:B,2,0))</f>
         <v/>
       </c>
-      <c r="P3" s="103"/>
+      <c r="P3" s="85"/>
       <c r="Q3" s="25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
-      <c r="J4" s="101"/>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="J4" s="83"/>
       <c r="O4" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P4" s="103"/>
+      <c r="P4" s="85"/>
       <c r="Q4" s="25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
-      <c r="J5" s="101"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="J5" s="83"/>
       <c r="O5" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P5" s="103"/>
+      <c r="P5" s="85"/>
       <c r="Q5" s="25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
-      <c r="J6" s="101"/>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="J6" s="83"/>
       <c r="O6" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P6" s="103"/>
+      <c r="P6" s="85"/>
       <c r="Q6" s="25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
-      <c r="J7" s="101"/>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="J7" s="83"/>
       <c r="O7" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P7" s="103"/>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="J8" s="101"/>
+      <c r="P7" s="85"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="J8" s="83"/>
       <c r="O8" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P8" s="103"/>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="J9" s="101"/>
+      <c r="P8" s="85"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="J9" s="83"/>
       <c r="O9" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P9" s="103"/>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="J10" s="101"/>
+      <c r="P9" s="85"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="J10" s="83"/>
       <c r="O10" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P10" s="103"/>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="J11" s="101"/>
+      <c r="P10" s="85"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="J11" s="83"/>
       <c r="O11" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P11" s="103"/>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="J12" s="101"/>
+      <c r="P11" s="85"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="J12" s="83"/>
       <c r="O12" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P12" s="103"/>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="J13" s="101"/>
+      <c r="P12" s="85"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="J13" s="83"/>
       <c r="O13" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P13" s="103"/>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="J14" s="101"/>
+      <c r="P13" s="85"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="J14" s="83"/>
       <c r="O14" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P14" s="103"/>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="J15" s="101"/>
+      <c r="P14" s="85"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="J15" s="83"/>
       <c r="O15" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P15" s="103"/>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="J16" s="101"/>
+      <c r="P15" s="85"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="J16" s="83"/>
       <c r="O16" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P16" s="103"/>
-    </row>
-    <row r="17" spans="10:16">
-      <c r="J17" s="101"/>
+      <c r="P16" s="85"/>
+    </row>
+    <row r="17" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J17" s="83"/>
       <c r="O17" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P17" s="103"/>
-    </row>
-    <row r="18" spans="10:16">
-      <c r="J18" s="101"/>
+      <c r="P17" s="85"/>
+    </row>
+    <row r="18" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J18" s="83"/>
       <c r="O18" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P18" s="103"/>
-    </row>
-    <row r="19" spans="10:16">
-      <c r="J19" s="101"/>
+      <c r="P18" s="85"/>
+    </row>
+    <row r="19" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J19" s="83"/>
       <c r="O19" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P19" s="103"/>
-    </row>
-    <row r="20" spans="10:16">
-      <c r="J20" s="101"/>
+      <c r="P19" s="85"/>
+    </row>
+    <row r="20" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J20" s="83"/>
       <c r="O20" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P20" s="103"/>
-    </row>
-    <row r="21" spans="10:16">
-      <c r="J21" s="101"/>
+      <c r="P20" s="85"/>
+    </row>
+    <row r="21" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J21" s="83"/>
       <c r="O21" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P21" s="103"/>
-    </row>
-    <row r="22" spans="10:16">
-      <c r="J22" s="101"/>
+      <c r="P21" s="85"/>
+    </row>
+    <row r="22" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J22" s="83"/>
       <c r="O22" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P22" s="103"/>
-    </row>
-    <row r="23" spans="10:16">
-      <c r="J23" s="101"/>
+      <c r="P22" s="85"/>
+    </row>
+    <row r="23" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J23" s="83"/>
       <c r="O23" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P23" s="103"/>
-    </row>
-    <row r="24" spans="10:16">
-      <c r="J24" s="101"/>
+      <c r="P23" s="85"/>
+    </row>
+    <row r="24" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J24" s="83"/>
       <c r="O24" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P24" s="103"/>
-    </row>
-    <row r="25" spans="10:16">
-      <c r="J25" s="101"/>
+      <c r="P24" s="85"/>
+    </row>
+    <row r="25" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J25" s="83"/>
       <c r="O25" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P25" s="103"/>
-    </row>
-    <row r="26" spans="10:16">
-      <c r="J26" s="101"/>
+      <c r="P25" s="85"/>
+    </row>
+    <row r="26" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J26" s="83"/>
       <c r="O26" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P26" s="103"/>
-    </row>
-    <row r="27" spans="10:16">
-      <c r="J27" s="101"/>
+      <c r="P26" s="85"/>
+    </row>
+    <row r="27" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J27" s="83"/>
       <c r="O27" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P27" s="103"/>
-    </row>
-    <row r="28" spans="10:16">
-      <c r="J28" s="101"/>
+      <c r="P27" s="85"/>
+    </row>
+    <row r="28" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J28" s="83"/>
       <c r="O28" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P28" s="103"/>
-    </row>
-    <row r="29" spans="10:16">
-      <c r="J29" s="101"/>
+      <c r="P28" s="85"/>
+    </row>
+    <row r="29" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J29" s="83"/>
       <c r="O29" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P29" s="103"/>
-    </row>
-    <row r="30" spans="10:16">
-      <c r="J30" s="101"/>
+      <c r="P29" s="85"/>
+    </row>
+    <row r="30" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J30" s="83"/>
       <c r="O30" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P30" s="103"/>
-    </row>
-    <row r="31" spans="10:16">
-      <c r="J31" s="101"/>
+      <c r="P30" s="85"/>
+    </row>
+    <row r="31" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J31" s="83"/>
       <c r="O31" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P31" s="103"/>
-    </row>
-    <row r="32" spans="10:16">
-      <c r="J32" s="101"/>
+      <c r="P31" s="85"/>
+    </row>
+    <row r="32" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J32" s="83"/>
       <c r="O32" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P32" s="103"/>
-    </row>
-    <row r="33" spans="10:20">
-      <c r="J33" s="101"/>
+      <c r="P32" s="85"/>
+    </row>
+    <row r="33" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J33" s="83"/>
       <c r="O33" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P33" s="103"/>
-    </row>
-    <row r="34" spans="10:20">
-      <c r="J34" s="101"/>
+      <c r="P33" s="85"/>
+    </row>
+    <row r="34" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J34" s="83"/>
       <c r="O34" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P34" s="103"/>
-    </row>
-    <row r="35" spans="10:20">
-      <c r="J35" s="101"/>
+      <c r="P34" s="85"/>
+    </row>
+    <row r="35" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J35" s="83"/>
       <c r="O35" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P35" s="103"/>
-    </row>
-    <row r="36" spans="10:20">
-      <c r="J36" s="101"/>
+      <c r="P35" s="85"/>
+    </row>
+    <row r="36" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J36" s="83"/>
       <c r="O36" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P36" s="103"/>
-    </row>
-    <row r="37" spans="10:20">
-      <c r="J37" s="101"/>
+      <c r="P36" s="85"/>
+    </row>
+    <row r="37" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J37" s="83"/>
       <c r="O37" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P37" s="103"/>
-    </row>
-    <row r="38" spans="10:20">
-      <c r="J38" s="101"/>
+      <c r="P37" s="85"/>
+    </row>
+    <row r="38" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J38" s="83"/>
       <c r="O38" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P38" s="103"/>
-    </row>
-    <row r="39" spans="10:20">
-      <c r="J39" s="101"/>
+      <c r="P38" s="85"/>
+    </row>
+    <row r="39" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J39" s="83"/>
       <c r="O39" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P39" s="103"/>
-    </row>
-    <row r="40" spans="10:20">
-      <c r="J40" s="101"/>
+      <c r="P39" s="85"/>
+    </row>
+    <row r="40" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J40" s="83"/>
       <c r="O40" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P40" s="103"/>
-    </row>
-    <row r="41" spans="10:20">
-      <c r="J41" s="101"/>
+      <c r="P40" s="85"/>
+    </row>
+    <row r="41" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J41" s="83"/>
       <c r="O41" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P41" s="103"/>
-    </row>
-    <row r="42" spans="10:20">
-      <c r="J42" s="101"/>
+      <c r="P41" s="85"/>
+    </row>
+    <row r="42" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J42" s="83"/>
       <c r="O42" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P42" s="103"/>
-    </row>
-    <row r="43" spans="10:20">
-      <c r="J43" s="101"/>
+      <c r="P42" s="85"/>
+    </row>
+    <row r="43" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J43" s="83"/>
       <c r="O43" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P43" s="103"/>
-    </row>
-    <row r="44" spans="10:20">
-      <c r="J44" s="101"/>
+      <c r="P43" s="85"/>
+    </row>
+    <row r="44" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J44" s="83"/>
       <c r="O44" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P44" s="103"/>
-    </row>
-    <row r="45" spans="10:20">
-      <c r="J45" s="101"/>
+      <c r="P44" s="85"/>
+    </row>
+    <row r="45" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J45" s="83"/>
       <c r="O45" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P45" s="103"/>
-    </row>
-    <row r="46" spans="10:20">
-      <c r="J46" s="101"/>
+      <c r="P45" s="85"/>
+    </row>
+    <row r="46" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J46" s="83"/>
       <c r="O46" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P46" s="103"/>
-    </row>
-    <row r="47" spans="10:20">
-      <c r="J47" s="101"/>
+      <c r="P46" s="85"/>
+    </row>
+    <row r="47" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J47" s="83"/>
       <c r="M47" s="29"/>
       <c r="O47" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P47" s="103"/>
+      <c r="P47" s="85"/>
       <c r="Q47" s="30"/>
       <c r="R47" s="30"/>
       <c r="S47" s="30"/>
       <c r="T47" s="30"/>
     </row>
-    <row r="48" spans="10:20">
-      <c r="J48" s="101"/>
+    <row r="48" spans="10:20" x14ac:dyDescent="0.4">
+      <c r="J48" s="83"/>
       <c r="O48" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P48" s="103"/>
-    </row>
-    <row r="49" spans="10:16">
-      <c r="J49" s="101"/>
+      <c r="P48" s="85"/>
+    </row>
+    <row r="49" spans="10:16" x14ac:dyDescent="0.4">
+      <c r="J49" s="83"/>
       <c r="O49" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P49" s="103"/>
-    </row>
-    <row r="50" spans="10:16">
+      <c r="P49" s="85"/>
+    </row>
+    <row r="50" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O50" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P50" s="103"/>
-    </row>
-    <row r="51" spans="10:16">
+      <c r="P50" s="85"/>
+    </row>
+    <row r="51" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O51" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P51" s="103"/>
-    </row>
-    <row r="52" spans="10:16">
+      <c r="P51" s="85"/>
+    </row>
+    <row r="52" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O52" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P52" s="103"/>
-    </row>
-    <row r="53" spans="10:16">
+      <c r="P52" s="85"/>
+    </row>
+    <row r="53" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O53" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P53" s="103"/>
-    </row>
-    <row r="54" spans="10:16">
+      <c r="P53" s="85"/>
+    </row>
+    <row r="54" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O54" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P54" s="103"/>
-    </row>
-    <row r="55" spans="10:16">
+      <c r="P54" s="85"/>
+    </row>
+    <row r="55" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O55" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P55" s="103"/>
-    </row>
-    <row r="56" spans="10:16">
+      <c r="P55" s="85"/>
+    </row>
+    <row r="56" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O56" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P56" s="103"/>
-    </row>
-    <row r="57" spans="10:16">
+      <c r="P56" s="85"/>
+    </row>
+    <row r="57" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O57" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P57" s="103"/>
-    </row>
-    <row r="58" spans="10:16">
+      <c r="P57" s="85"/>
+    </row>
+    <row r="58" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O58" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P58" s="103"/>
-    </row>
-    <row r="59" spans="10:16">
+      <c r="P58" s="85"/>
+    </row>
+    <row r="59" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O59" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P59" s="103"/>
-    </row>
-    <row r="60" spans="10:16">
+      <c r="P59" s="85"/>
+    </row>
+    <row r="60" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O60" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P60" s="103"/>
-    </row>
-    <row r="61" spans="10:16">
+      <c r="P60" s="85"/>
+    </row>
+    <row r="61" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O61" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P61" s="103"/>
-    </row>
-    <row r="62" spans="10:16">
+      <c r="P61" s="85"/>
+    </row>
+    <row r="62" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O62" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P62" s="103"/>
-    </row>
-    <row r="63" spans="10:16">
+      <c r="P62" s="85"/>
+    </row>
+    <row r="63" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O63" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P63" s="103"/>
-    </row>
-    <row r="64" spans="10:16">
+      <c r="P63" s="85"/>
+    </row>
+    <row r="64" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O64" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P64" s="103"/>
-    </row>
-    <row r="65" spans="15:16">
+      <c r="P64" s="85"/>
+    </row>
+    <row r="65" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O65" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P65" s="103"/>
-    </row>
-    <row r="66" spans="15:16">
+      <c r="P65" s="85"/>
+    </row>
+    <row r="66" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O66" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P66" s="103"/>
-    </row>
-    <row r="67" spans="15:16">
+      <c r="P66" s="85"/>
+    </row>
+    <row r="67" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O67" s="23" t="str">
         <f t="shared" ref="O67:O113" si="1">IF(ISNA(VLOOKUP(G67,A:B,2,0)),"",VLOOKUP(G67,A:B,2,0))</f>
         <v/>
       </c>
-      <c r="P67" s="103"/>
-    </row>
-    <row r="68" spans="15:16">
+      <c r="P67" s="85"/>
+    </row>
+    <row r="68" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O68" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P68" s="103"/>
-    </row>
-    <row r="69" spans="15:16">
+      <c r="P68" s="85"/>
+    </row>
+    <row r="69" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O69" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P69" s="103"/>
-    </row>
-    <row r="70" spans="15:16">
+      <c r="P69" s="85"/>
+    </row>
+    <row r="70" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O70" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P70" s="103"/>
-    </row>
-    <row r="71" spans="15:16">
+      <c r="P70" s="85"/>
+    </row>
+    <row r="71" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O71" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P71" s="103"/>
-    </row>
-    <row r="72" spans="15:16">
+      <c r="P71" s="85"/>
+    </row>
+    <row r="72" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O72" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P72" s="103"/>
-    </row>
-    <row r="73" spans="15:16">
+      <c r="P72" s="85"/>
+    </row>
+    <row r="73" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O73" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P73" s="103"/>
-    </row>
-    <row r="74" spans="15:16">
+      <c r="P73" s="85"/>
+    </row>
+    <row r="74" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O74" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P74" s="103"/>
-    </row>
-    <row r="75" spans="15:16">
+      <c r="P74" s="85"/>
+    </row>
+    <row r="75" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O75" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P75" s="103"/>
-    </row>
-    <row r="76" spans="15:16">
+      <c r="P75" s="85"/>
+    </row>
+    <row r="76" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O76" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P76" s="103"/>
-    </row>
-    <row r="77" spans="15:16">
+      <c r="P76" s="85"/>
+    </row>
+    <row r="77" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O77" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P77" s="103"/>
-    </row>
-    <row r="78" spans="15:16">
+      <c r="P77" s="85"/>
+    </row>
+    <row r="78" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O78" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P78" s="103"/>
-    </row>
-    <row r="79" spans="15:16">
+      <c r="P78" s="85"/>
+    </row>
+    <row r="79" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O79" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P79" s="103"/>
-    </row>
-    <row r="80" spans="15:16">
+      <c r="P79" s="85"/>
+    </row>
+    <row r="80" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O80" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P80" s="103"/>
-    </row>
-    <row r="81" spans="15:16">
+      <c r="P80" s="85"/>
+    </row>
+    <row r="81" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O81" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P81" s="103"/>
-    </row>
-    <row r="82" spans="15:16">
+      <c r="P81" s="85"/>
+    </row>
+    <row r="82" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O82" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P82" s="103"/>
-    </row>
-    <row r="83" spans="15:16">
+      <c r="P82" s="85"/>
+    </row>
+    <row r="83" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O83" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P83" s="103"/>
-    </row>
-    <row r="84" spans="15:16">
+      <c r="P83" s="85"/>
+    </row>
+    <row r="84" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O84" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P84" s="103"/>
-    </row>
-    <row r="85" spans="15:16">
+      <c r="P84" s="85"/>
+    </row>
+    <row r="85" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O85" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P85" s="103"/>
-    </row>
-    <row r="86" spans="15:16">
+      <c r="P85" s="85"/>
+    </row>
+    <row r="86" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O86" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P86" s="103"/>
-    </row>
-    <row r="87" spans="15:16">
+      <c r="P86" s="85"/>
+    </row>
+    <row r="87" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O87" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P87" s="103"/>
-    </row>
-    <row r="88" spans="15:16">
+      <c r="P87" s="85"/>
+    </row>
+    <row r="88" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O88" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P88" s="103"/>
-    </row>
-    <row r="89" spans="15:16">
+      <c r="P88" s="85"/>
+    </row>
+    <row r="89" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O89" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P89" s="103"/>
-    </row>
-    <row r="90" spans="15:16">
+      <c r="P89" s="85"/>
+    </row>
+    <row r="90" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O90" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P90" s="103"/>
-    </row>
-    <row r="91" spans="15:16">
+      <c r="P90" s="85"/>
+    </row>
+    <row r="91" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O91" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P91" s="103"/>
-    </row>
-    <row r="92" spans="15:16">
+      <c r="P91" s="85"/>
+    </row>
+    <row r="92" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O92" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P92" s="103"/>
-    </row>
-    <row r="93" spans="15:16">
+      <c r="P92" s="85"/>
+    </row>
+    <row r="93" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O93" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P93" s="103"/>
-    </row>
-    <row r="94" spans="15:16">
+      <c r="P93" s="85"/>
+    </row>
+    <row r="94" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O94" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P94" s="103"/>
-    </row>
-    <row r="95" spans="15:16">
+      <c r="P94" s="85"/>
+    </row>
+    <row r="95" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O95" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P95" s="103"/>
-    </row>
-    <row r="96" spans="15:16">
+      <c r="P95" s="85"/>
+    </row>
+    <row r="96" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O96" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P96" s="103"/>
-    </row>
-    <row r="97" spans="15:16">
+      <c r="P96" s="85"/>
+    </row>
+    <row r="97" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O97" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P97" s="103"/>
-    </row>
-    <row r="98" spans="15:16">
+      <c r="P97" s="85"/>
+    </row>
+    <row r="98" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O98" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P98" s="103"/>
-    </row>
-    <row r="99" spans="15:16">
+      <c r="P98" s="85"/>
+    </row>
+    <row r="99" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O99" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P99" s="103"/>
-    </row>
-    <row r="100" spans="15:16">
+      <c r="P99" s="85"/>
+    </row>
+    <row r="100" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O100" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P100" s="103"/>
-    </row>
-    <row r="101" spans="15:16">
+      <c r="P100" s="85"/>
+    </row>
+    <row r="101" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O101" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P101" s="103"/>
-    </row>
-    <row r="102" spans="15:16">
+      <c r="P101" s="85"/>
+    </row>
+    <row r="102" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O102" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P102" s="103"/>
-    </row>
-    <row r="103" spans="15:16">
+      <c r="P102" s="85"/>
+    </row>
+    <row r="103" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O103" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P103" s="103"/>
-    </row>
-    <row r="104" spans="15:16">
+      <c r="P103" s="85"/>
+    </row>
+    <row r="104" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O104" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P104" s="103"/>
-    </row>
-    <row r="105" spans="15:16">
+      <c r="P104" s="85"/>
+    </row>
+    <row r="105" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O105" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P105" s="103"/>
-    </row>
-    <row r="106" spans="15:16">
+      <c r="P105" s="85"/>
+    </row>
+    <row r="106" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O106" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P106" s="103"/>
-    </row>
-    <row r="107" spans="15:16">
+      <c r="P106" s="85"/>
+    </row>
+    <row r="107" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O107" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P107" s="103"/>
-    </row>
-    <row r="108" spans="15:16">
+      <c r="P107" s="85"/>
+    </row>
+    <row r="108" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O108" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P108" s="103"/>
-    </row>
-    <row r="109" spans="15:16">
+      <c r="P108" s="85"/>
+    </row>
+    <row r="109" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O109" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P109" s="103"/>
-    </row>
-    <row r="110" spans="15:16">
+      <c r="P109" s="85"/>
+    </row>
+    <row r="110" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O110" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P110" s="103"/>
-    </row>
-    <row r="111" spans="15:16">
+      <c r="P110" s="85"/>
+    </row>
+    <row r="111" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O111" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P111" s="103"/>
-    </row>
-    <row r="112" spans="15:16">
+      <c r="P111" s="85"/>
+    </row>
+    <row r="112" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O112" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P112" s="103"/>
-    </row>
-    <row r="113" spans="15:16">
+      <c r="P112" s="85"/>
+    </row>
+    <row r="113" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O113" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P113" s="103"/>
-    </row>
-    <row r="114" spans="15:16">
-      <c r="P114" s="103"/>
-    </row>
-    <row r="115" spans="15:16">
-      <c r="P115" s="103"/>
-    </row>
-    <row r="116" spans="15:16">
-      <c r="P116" s="103"/>
-    </row>
-    <row r="117" spans="15:16">
-      <c r="P117" s="103"/>
+      <c r="P113" s="85"/>
+    </row>
+    <row r="114" spans="15:16" x14ac:dyDescent="0.4">
+      <c r="P114" s="85"/>
+    </row>
+    <row r="115" spans="15:16" x14ac:dyDescent="0.4">
+      <c r="P115" s="85"/>
+    </row>
+    <row r="116" spans="15:16" x14ac:dyDescent="0.4">
+      <c r="P116" s="85"/>
+    </row>
+    <row r="117" spans="15:16" x14ac:dyDescent="0.4">
+      <c r="P117" s="85"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Auto-committed on 2022/05/20 週五 16:33:38.16
</commit_message>
<xml_diff>
--- a/Program/Other/LM057_底稿_表14-5、14-6_會計部申報表.xlsx
+++ b/Program/Other/LM057_底稿_表14-5、14-6_會計部申報表.xlsx
@@ -1654,7 +1654,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1887,9 +1887,6 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1967,6 +1964,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2389,10 +2392,10 @@
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="87"/>
+      <c r="C4" s="86"/>
       <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
@@ -2401,7 +2404,7 @@
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="87" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2413,7 +2416,7 @@
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="89"/>
+      <c r="B6" s="88"/>
       <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
@@ -2423,7 +2426,7 @@
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="89"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
@@ -2433,7 +2436,7 @@
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="89"/>
+      <c r="B8" s="88"/>
       <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
@@ -2443,7 +2446,7 @@
       <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" s="89"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
@@ -2453,7 +2456,7 @@
       <c r="A10" s="1">
         <v>6</v>
       </c>
-      <c r="B10" s="89"/>
+      <c r="B10" s="88"/>
       <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
@@ -2463,7 +2466,7 @@
       <c r="A11" s="1">
         <v>7</v>
       </c>
-      <c r="B11" s="89"/>
+      <c r="B11" s="88"/>
       <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
@@ -2473,7 +2476,7 @@
       <c r="A12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="90" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -2488,7 +2491,7 @@
       <c r="A13" s="1">
         <v>9</v>
       </c>
-      <c r="B13" s="92"/>
+      <c r="B13" s="91"/>
       <c r="C13" s="12" t="s">
         <v>0</v>
       </c>
@@ -2501,7 +2504,7 @@
       <c r="A14" s="1">
         <v>10</v>
       </c>
-      <c r="B14" s="93"/>
+      <c r="B14" s="92"/>
       <c r="C14" s="12" t="s">
         <v>1</v>
       </c>
@@ -2514,10 +2517,10 @@
       <c r="A15" s="1">
         <v>11</v>
       </c>
-      <c r="B15" s="90" t="s">
+      <c r="B15" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="90"/>
+      <c r="C15" s="89"/>
       <c r="D15" s="17">
         <f>'14-5申報表'!D18</f>
         <v>0</v>
@@ -2527,40 +2530,40 @@
       <c r="A16" s="1">
         <v>12</v>
       </c>
-      <c r="B16" s="94" t="s">
+      <c r="B16" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="95"/>
+      <c r="C16" s="94"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>13</v>
       </c>
-      <c r="B17" s="96" t="s">
+      <c r="B17" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="97"/>
+      <c r="C17" s="96"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>14</v>
       </c>
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="97"/>
+      <c r="C18" s="96"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>15</v>
       </c>
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="95"/>
+      <c r="C19" s="94"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="19.5" x14ac:dyDescent="0.4">
@@ -2590,20 +2593,20 @@
       <c r="A22" s="1">
         <v>18</v>
       </c>
-      <c r="B22" s="88" t="s">
+      <c r="B22" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="88"/>
+      <c r="C22" s="87"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>19</v>
       </c>
-      <c r="B23" s="88" t="s">
+      <c r="B23" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="88"/>
+      <c r="C23" s="87"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:5" ht="19.5" x14ac:dyDescent="0.4">
@@ -2741,10 +2744,10 @@
       <c r="A4" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="99" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="101"/>
+      <c r="C4" s="100"/>
       <c r="D4" s="63" t="s">
         <v>17</v>
       </c>
@@ -2753,7 +2756,7 @@
       <c r="A5" s="43">
         <v>1</v>
       </c>
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="101" t="s">
         <v>82</v>
       </c>
       <c r="C5" s="52" t="s">
@@ -2767,7 +2770,7 @@
       <c r="A6" s="43">
         <v>2</v>
       </c>
-      <c r="B6" s="103"/>
+      <c r="B6" s="102"/>
       <c r="C6" s="52" t="s">
         <v>80</v>
       </c>
@@ -2783,7 +2786,7 @@
       <c r="A7" s="43">
         <v>3</v>
       </c>
-      <c r="B7" s="103"/>
+      <c r="B7" s="102"/>
       <c r="C7" s="62" t="s">
         <v>78</v>
       </c>
@@ -2797,7 +2800,7 @@
       <c r="A8" s="43">
         <v>4</v>
       </c>
-      <c r="B8" s="103"/>
+      <c r="B8" s="102"/>
       <c r="C8" s="57" t="s">
         <v>77</v>
       </c>
@@ -2811,7 +2814,7 @@
       <c r="A9" s="43">
         <v>5</v>
       </c>
-      <c r="B9" s="103"/>
+      <c r="B9" s="102"/>
       <c r="C9" s="49" t="s">
         <v>76</v>
       </c>
@@ -2828,7 +2831,7 @@
       <c r="A10" s="43">
         <v>6</v>
       </c>
-      <c r="B10" s="102" t="s">
+      <c r="B10" s="101" t="s">
         <v>75</v>
       </c>
       <c r="C10" s="57" t="s">
@@ -2844,7 +2847,7 @@
       <c r="A11" s="43">
         <v>7</v>
       </c>
-      <c r="B11" s="104"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="57" t="s">
         <v>73</v>
       </c>
@@ -2858,7 +2861,7 @@
       <c r="A12" s="43">
         <v>8</v>
       </c>
-      <c r="B12" s="104"/>
+      <c r="B12" s="103"/>
       <c r="C12" s="57" t="s">
         <v>72</v>
       </c>
@@ -2872,7 +2875,7 @@
       <c r="A13" s="43">
         <v>9</v>
       </c>
-      <c r="B13" s="104"/>
+      <c r="B13" s="103"/>
       <c r="C13" s="52" t="s">
         <v>71</v>
       </c>
@@ -2886,7 +2889,7 @@
       <c r="A14" s="43">
         <v>10</v>
       </c>
-      <c r="B14" s="104"/>
+      <c r="B14" s="103"/>
       <c r="C14" s="52" t="s">
         <v>70</v>
       </c>
@@ -2900,7 +2903,7 @@
       <c r="A15" s="43">
         <v>11</v>
       </c>
-      <c r="B15" s="104"/>
+      <c r="B15" s="103"/>
       <c r="C15" s="52" t="s">
         <v>69</v>
       </c>
@@ -2916,7 +2919,7 @@
       <c r="A16" s="43">
         <v>12</v>
       </c>
-      <c r="B16" s="104"/>
+      <c r="B16" s="103"/>
       <c r="C16" s="52" t="s">
         <v>67</v>
       </c>
@@ -2932,7 +2935,7 @@
       <c r="A17" s="43">
         <v>13</v>
       </c>
-      <c r="B17" s="104"/>
+      <c r="B17" s="103"/>
       <c r="C17" s="49" t="s">
         <v>65</v>
       </c>
@@ -3024,12 +3027,12 @@
       </c>
     </row>
     <row r="24" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="98" t="s">
+      <c r="A24" s="97" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="99"/>
-      <c r="C24" s="99"/>
-      <c r="D24" s="99"/>
+      <c r="B24" s="98"/>
+      <c r="C24" s="98"/>
+      <c r="D24" s="98"/>
       <c r="F24" s="38"/>
       <c r="G24" s="37"/>
       <c r="H24"/>
@@ -3123,7 +3126,7 @@
   <dimension ref="A1:T117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -3131,12 +3134,13 @@
     <col min="1" max="1" width="7.90625" style="26" customWidth="1"/>
     <col min="2" max="2" width="5.6328125" style="26" customWidth="1"/>
     <col min="3" max="3" width="9" style="26" customWidth="1"/>
-    <col min="4" max="4" width="10" style="81" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="80" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="6" style="82" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.54296875" style="86" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6328125" style="84" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="80" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" style="79" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.90625" style="81" customWidth="1"/>
+    <col min="7" max="8" width="6" style="81" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" style="85" customWidth="1"/>
+    <col min="10" max="10" width="12.6328125" style="83" customWidth="1"/>
+    <col min="11" max="11" width="16.90625" style="79" customWidth="1"/>
     <col min="12" max="12" width="8.81640625" style="70" customWidth="1"/>
     <col min="13" max="13" width="6" style="28" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.26953125" style="24" bestFit="1" customWidth="1"/>
@@ -3144,7 +3148,7 @@
     <col min="17" max="16384" width="8.90625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" s="78" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="71"/>
       <c r="B1" s="72"/>
       <c r="C1" s="73">
@@ -3156,7 +3160,7 @@
       <c r="E1" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="76" t="s">
+      <c r="F1" s="104" t="s">
         <v>39</v>
       </c>
       <c r="G1" s="76" t="s">
@@ -3166,7 +3170,7 @@
         <v>41</v>
       </c>
       <c r="I1" s="22">
-        <f>COUNT(I2:I500)</f>
+        <f>SUBTOTAL(3,I2:I500)</f>
         <v>0</v>
       </c>
       <c r="J1" s="69">
@@ -3176,7 +3180,7 @@
       <c r="K1" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="78" t="s">
+      <c r="L1" s="105" t="s">
         <v>93</v>
       </c>
       <c r="M1" s="21" t="s">
@@ -3194,869 +3198,869 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="C2" s="27"/>
-      <c r="D2" s="80"/>
-      <c r="J2" s="83"/>
+      <c r="D2" s="79"/>
+      <c r="J2" s="82"/>
       <c r="O2" s="23" t="str">
         <f>IF(ISNA(VLOOKUP(G2,A:B,2,0)),"",VLOOKUP(G2,A:B,2,0))</f>
         <v/>
       </c>
-      <c r="P2" s="85"/>
+      <c r="P2" s="84"/>
       <c r="Q2" s="25" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="J3" s="83"/>
+      <c r="J3" s="82"/>
       <c r="O3" s="23" t="str">
         <f t="shared" ref="O3:O66" si="0">IF(ISNA(VLOOKUP(G3,A:B,2,0)),"",VLOOKUP(G3,A:B,2,0))</f>
         <v/>
       </c>
-      <c r="P3" s="85"/>
+      <c r="P3" s="84"/>
       <c r="Q3" s="25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="J4" s="83"/>
+      <c r="J4" s="82"/>
       <c r="O4" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P4" s="85"/>
+      <c r="P4" s="84"/>
       <c r="Q4" s="25" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="J5" s="83"/>
+      <c r="J5" s="82"/>
       <c r="O5" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P5" s="85"/>
+      <c r="P5" s="84"/>
       <c r="Q5" s="25" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="J6" s="83"/>
+      <c r="J6" s="82"/>
       <c r="O6" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P6" s="85"/>
+      <c r="P6" s="84"/>
       <c r="Q6" s="25" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="J7" s="83"/>
+      <c r="J7" s="82"/>
       <c r="O7" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P7" s="85"/>
+      <c r="P7" s="84"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="J8" s="83"/>
+      <c r="J8" s="82"/>
       <c r="O8" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P8" s="85"/>
+      <c r="P8" s="84"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="J9" s="83"/>
+      <c r="J9" s="82"/>
       <c r="O9" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P9" s="85"/>
+      <c r="P9" s="84"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="J10" s="83"/>
+      <c r="J10" s="82"/>
       <c r="O10" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P10" s="85"/>
+      <c r="P10" s="84"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="J11" s="83"/>
+      <c r="J11" s="82"/>
       <c r="O11" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P11" s="85"/>
+      <c r="P11" s="84"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="J12" s="83"/>
+      <c r="J12" s="82"/>
       <c r="O12" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P12" s="85"/>
+      <c r="P12" s="84"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="J13" s="83"/>
+      <c r="J13" s="82"/>
       <c r="O13" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P13" s="85"/>
+      <c r="P13" s="84"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="J14" s="83"/>
+      <c r="J14" s="82"/>
       <c r="O14" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P14" s="85"/>
+      <c r="P14" s="84"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="J15" s="83"/>
+      <c r="J15" s="82"/>
       <c r="O15" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P15" s="85"/>
+      <c r="P15" s="84"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="J16" s="83"/>
+      <c r="J16" s="82"/>
       <c r="O16" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P16" s="85"/>
+      <c r="P16" s="84"/>
     </row>
     <row r="17" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J17" s="83"/>
+      <c r="J17" s="82"/>
       <c r="O17" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P17" s="85"/>
+      <c r="P17" s="84"/>
     </row>
     <row r="18" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J18" s="83"/>
+      <c r="J18" s="82"/>
       <c r="O18" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P18" s="85"/>
+      <c r="P18" s="84"/>
     </row>
     <row r="19" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J19" s="83"/>
+      <c r="J19" s="82"/>
       <c r="O19" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P19" s="85"/>
+      <c r="P19" s="84"/>
     </row>
     <row r="20" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J20" s="83"/>
+      <c r="J20" s="82"/>
       <c r="O20" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P20" s="85"/>
+      <c r="P20" s="84"/>
     </row>
     <row r="21" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J21" s="83"/>
+      <c r="J21" s="82"/>
       <c r="O21" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P21" s="85"/>
+      <c r="P21" s="84"/>
     </row>
     <row r="22" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J22" s="83"/>
+      <c r="J22" s="82"/>
       <c r="O22" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P22" s="85"/>
+      <c r="P22" s="84"/>
     </row>
     <row r="23" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J23" s="83"/>
+      <c r="J23" s="82"/>
       <c r="O23" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P23" s="85"/>
+      <c r="P23" s="84"/>
     </row>
     <row r="24" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J24" s="83"/>
+      <c r="J24" s="82"/>
       <c r="O24" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P24" s="85"/>
+      <c r="P24" s="84"/>
     </row>
     <row r="25" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J25" s="83"/>
+      <c r="J25" s="82"/>
       <c r="O25" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P25" s="85"/>
+      <c r="P25" s="84"/>
     </row>
     <row r="26" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J26" s="83"/>
+      <c r="J26" s="82"/>
       <c r="O26" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P26" s="85"/>
+      <c r="P26" s="84"/>
     </row>
     <row r="27" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J27" s="83"/>
+      <c r="J27" s="82"/>
       <c r="O27" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P27" s="85"/>
+      <c r="P27" s="84"/>
     </row>
     <row r="28" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J28" s="83"/>
+      <c r="J28" s="82"/>
       <c r="O28" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P28" s="85"/>
+      <c r="P28" s="84"/>
     </row>
     <row r="29" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J29" s="83"/>
+      <c r="J29" s="82"/>
       <c r="O29" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P29" s="85"/>
+      <c r="P29" s="84"/>
     </row>
     <row r="30" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J30" s="83"/>
+      <c r="J30" s="82"/>
       <c r="O30" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P30" s="85"/>
+      <c r="P30" s="84"/>
     </row>
     <row r="31" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J31" s="83"/>
+      <c r="J31" s="82"/>
       <c r="O31" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P31" s="85"/>
+      <c r="P31" s="84"/>
     </row>
     <row r="32" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J32" s="83"/>
+      <c r="J32" s="82"/>
       <c r="O32" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P32" s="85"/>
+      <c r="P32" s="84"/>
     </row>
     <row r="33" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J33" s="83"/>
+      <c r="J33" s="82"/>
       <c r="O33" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P33" s="85"/>
+      <c r="P33" s="84"/>
     </row>
     <row r="34" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J34" s="83"/>
+      <c r="J34" s="82"/>
       <c r="O34" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P34" s="85"/>
+      <c r="P34" s="84"/>
     </row>
     <row r="35" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J35" s="83"/>
+      <c r="J35" s="82"/>
       <c r="O35" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P35" s="85"/>
+      <c r="P35" s="84"/>
     </row>
     <row r="36" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J36" s="83"/>
+      <c r="J36" s="82"/>
       <c r="O36" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P36" s="85"/>
+      <c r="P36" s="84"/>
     </row>
     <row r="37" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J37" s="83"/>
+      <c r="J37" s="82"/>
       <c r="O37" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P37" s="85"/>
+      <c r="P37" s="84"/>
     </row>
     <row r="38" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J38" s="83"/>
+      <c r="J38" s="82"/>
       <c r="O38" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P38" s="85"/>
+      <c r="P38" s="84"/>
     </row>
     <row r="39" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J39" s="83"/>
+      <c r="J39" s="82"/>
       <c r="O39" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P39" s="85"/>
+      <c r="P39" s="84"/>
     </row>
     <row r="40" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J40" s="83"/>
+      <c r="J40" s="82"/>
       <c r="O40" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P40" s="85"/>
+      <c r="P40" s="84"/>
     </row>
     <row r="41" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J41" s="83"/>
+      <c r="J41" s="82"/>
       <c r="O41" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P41" s="85"/>
+      <c r="P41" s="84"/>
     </row>
     <row r="42" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J42" s="83"/>
+      <c r="J42" s="82"/>
       <c r="O42" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P42" s="85"/>
+      <c r="P42" s="84"/>
     </row>
     <row r="43" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J43" s="83"/>
+      <c r="J43" s="82"/>
       <c r="O43" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P43" s="85"/>
+      <c r="P43" s="84"/>
     </row>
     <row r="44" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J44" s="83"/>
+      <c r="J44" s="82"/>
       <c r="O44" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P44" s="85"/>
+      <c r="P44" s="84"/>
     </row>
     <row r="45" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J45" s="83"/>
+      <c r="J45" s="82"/>
       <c r="O45" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P45" s="85"/>
+      <c r="P45" s="84"/>
     </row>
     <row r="46" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J46" s="83"/>
+      <c r="J46" s="82"/>
       <c r="O46" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P46" s="85"/>
+      <c r="P46" s="84"/>
     </row>
     <row r="47" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J47" s="83"/>
+      <c r="J47" s="82"/>
       <c r="M47" s="29"/>
       <c r="O47" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P47" s="85"/>
+      <c r="P47" s="84"/>
       <c r="Q47" s="30"/>
       <c r="R47" s="30"/>
       <c r="S47" s="30"/>
       <c r="T47" s="30"/>
     </row>
     <row r="48" spans="10:20" x14ac:dyDescent="0.4">
-      <c r="J48" s="83"/>
+      <c r="J48" s="82"/>
       <c r="O48" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P48" s="85"/>
+      <c r="P48" s="84"/>
     </row>
     <row r="49" spans="10:16" x14ac:dyDescent="0.4">
-      <c r="J49" s="83"/>
+      <c r="J49" s="82"/>
       <c r="O49" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P49" s="85"/>
+      <c r="P49" s="84"/>
     </row>
     <row r="50" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O50" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P50" s="85"/>
+      <c r="P50" s="84"/>
     </row>
     <row r="51" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O51" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P51" s="85"/>
+      <c r="P51" s="84"/>
     </row>
     <row r="52" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O52" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P52" s="85"/>
+      <c r="P52" s="84"/>
     </row>
     <row r="53" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O53" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P53" s="85"/>
+      <c r="P53" s="84"/>
     </row>
     <row r="54" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O54" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P54" s="85"/>
+      <c r="P54" s="84"/>
     </row>
     <row r="55" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O55" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P55" s="85"/>
+      <c r="P55" s="84"/>
     </row>
     <row r="56" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O56" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P56" s="85"/>
+      <c r="P56" s="84"/>
     </row>
     <row r="57" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O57" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P57" s="85"/>
+      <c r="P57" s="84"/>
     </row>
     <row r="58" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O58" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P58" s="85"/>
+      <c r="P58" s="84"/>
     </row>
     <row r="59" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O59" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P59" s="85"/>
+      <c r="P59" s="84"/>
     </row>
     <row r="60" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O60" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P60" s="85"/>
+      <c r="P60" s="84"/>
     </row>
     <row r="61" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O61" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P61" s="85"/>
+      <c r="P61" s="84"/>
     </row>
     <row r="62" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O62" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P62" s="85"/>
+      <c r="P62" s="84"/>
     </row>
     <row r="63" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O63" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P63" s="85"/>
+      <c r="P63" s="84"/>
     </row>
     <row r="64" spans="10:16" x14ac:dyDescent="0.4">
       <c r="O64" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P64" s="85"/>
+      <c r="P64" s="84"/>
     </row>
     <row r="65" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O65" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P65" s="85"/>
+      <c r="P65" s="84"/>
     </row>
     <row r="66" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O66" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P66" s="85"/>
+      <c r="P66" s="84"/>
     </row>
     <row r="67" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O67" s="23" t="str">
         <f t="shared" ref="O67:O113" si="1">IF(ISNA(VLOOKUP(G67,A:B,2,0)),"",VLOOKUP(G67,A:B,2,0))</f>
         <v/>
       </c>
-      <c r="P67" s="85"/>
+      <c r="P67" s="84"/>
     </row>
     <row r="68" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O68" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P68" s="85"/>
+      <c r="P68" s="84"/>
     </row>
     <row r="69" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O69" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P69" s="85"/>
+      <c r="P69" s="84"/>
     </row>
     <row r="70" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O70" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P70" s="85"/>
+      <c r="P70" s="84"/>
     </row>
     <row r="71" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O71" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P71" s="85"/>
+      <c r="P71" s="84"/>
     </row>
     <row r="72" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O72" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P72" s="85"/>
+      <c r="P72" s="84"/>
     </row>
     <row r="73" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O73" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P73" s="85"/>
+      <c r="P73" s="84"/>
     </row>
     <row r="74" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O74" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P74" s="85"/>
+      <c r="P74" s="84"/>
     </row>
     <row r="75" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O75" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P75" s="85"/>
+      <c r="P75" s="84"/>
     </row>
     <row r="76" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O76" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P76" s="85"/>
+      <c r="P76" s="84"/>
     </row>
     <row r="77" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O77" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P77" s="85"/>
+      <c r="P77" s="84"/>
     </row>
     <row r="78" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O78" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P78" s="85"/>
+      <c r="P78" s="84"/>
     </row>
     <row r="79" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O79" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P79" s="85"/>
+      <c r="P79" s="84"/>
     </row>
     <row r="80" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O80" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P80" s="85"/>
+      <c r="P80" s="84"/>
     </row>
     <row r="81" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O81" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P81" s="85"/>
+      <c r="P81" s="84"/>
     </row>
     <row r="82" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O82" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P82" s="85"/>
+      <c r="P82" s="84"/>
     </row>
     <row r="83" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O83" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P83" s="85"/>
+      <c r="P83" s="84"/>
     </row>
     <row r="84" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O84" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P84" s="85"/>
+      <c r="P84" s="84"/>
     </row>
     <row r="85" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O85" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P85" s="85"/>
+      <c r="P85" s="84"/>
     </row>
     <row r="86" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O86" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P86" s="85"/>
+      <c r="P86" s="84"/>
     </row>
     <row r="87" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O87" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P87" s="85"/>
+      <c r="P87" s="84"/>
     </row>
     <row r="88" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O88" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P88" s="85"/>
+      <c r="P88" s="84"/>
     </row>
     <row r="89" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O89" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P89" s="85"/>
+      <c r="P89" s="84"/>
     </row>
     <row r="90" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O90" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P90" s="85"/>
+      <c r="P90" s="84"/>
     </row>
     <row r="91" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O91" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P91" s="85"/>
+      <c r="P91" s="84"/>
     </row>
     <row r="92" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O92" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P92" s="85"/>
+      <c r="P92" s="84"/>
     </row>
     <row r="93" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O93" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P93" s="85"/>
+      <c r="P93" s="84"/>
     </row>
     <row r="94" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O94" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P94" s="85"/>
+      <c r="P94" s="84"/>
     </row>
     <row r="95" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O95" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P95" s="85"/>
+      <c r="P95" s="84"/>
     </row>
     <row r="96" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O96" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P96" s="85"/>
+      <c r="P96" s="84"/>
     </row>
     <row r="97" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O97" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P97" s="85"/>
+      <c r="P97" s="84"/>
     </row>
     <row r="98" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O98" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P98" s="85"/>
+      <c r="P98" s="84"/>
     </row>
     <row r="99" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O99" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P99" s="85"/>
+      <c r="P99" s="84"/>
     </row>
     <row r="100" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O100" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P100" s="85"/>
+      <c r="P100" s="84"/>
     </row>
     <row r="101" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O101" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P101" s="85"/>
+      <c r="P101" s="84"/>
     </row>
     <row r="102" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O102" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P102" s="85"/>
+      <c r="P102" s="84"/>
     </row>
     <row r="103" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O103" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P103" s="85"/>
+      <c r="P103" s="84"/>
     </row>
     <row r="104" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O104" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P104" s="85"/>
+      <c r="P104" s="84"/>
     </row>
     <row r="105" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O105" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P105" s="85"/>
+      <c r="P105" s="84"/>
     </row>
     <row r="106" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O106" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P106" s="85"/>
+      <c r="P106" s="84"/>
     </row>
     <row r="107" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O107" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P107" s="85"/>
+      <c r="P107" s="84"/>
     </row>
     <row r="108" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O108" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P108" s="85"/>
+      <c r="P108" s="84"/>
     </row>
     <row r="109" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O109" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P109" s="85"/>
+      <c r="P109" s="84"/>
     </row>
     <row r="110" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O110" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P110" s="85"/>
+      <c r="P110" s="84"/>
     </row>
     <row r="111" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O111" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P111" s="85"/>
+      <c r="P111" s="84"/>
     </row>
     <row r="112" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O112" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P112" s="85"/>
+      <c r="P112" s="84"/>
     </row>
     <row r="113" spans="15:16" x14ac:dyDescent="0.4">
       <c r="O113" s="23" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P113" s="85"/>
+      <c r="P113" s="84"/>
     </row>
     <row r="114" spans="15:16" x14ac:dyDescent="0.4">
-      <c r="P114" s="85"/>
+      <c r="P114" s="84"/>
     </row>
     <row r="115" spans="15:16" x14ac:dyDescent="0.4">
-      <c r="P115" s="85"/>
+      <c r="P115" s="84"/>
     </row>
     <row r="116" spans="15:16" x14ac:dyDescent="0.4">
-      <c r="P116" s="85"/>
+      <c r="P116" s="84"/>
     </row>
     <row r="117" spans="15:16" x14ac:dyDescent="0.4">
-      <c r="P117" s="85"/>
+      <c r="P117" s="84"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>